<commit_message>
tweaking Ne fits to not need intensities input from user (just sigma)
</commit_message>
<xml_diff>
--- a/docs/Examples/Diad_Fitting_Nov22nd2022/Medium_Diads.xlsx
+++ b/docs/Examples/Diad_Fitting_Nov22nd2022/Medium_Diads.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="74">
   <si>
     <t>filename</t>
   </si>
@@ -106,66 +106,57 @@
     <t>C13_Sigma</t>
   </si>
   <si>
-    <t>POC10</t>
-  </si>
-  <si>
-    <t>POC11</t>
-  </si>
-  <si>
-    <t>POC12</t>
-  </si>
-  <si>
-    <t>POC13</t>
-  </si>
-  <si>
-    <t>POC14</t>
-  </si>
-  <si>
-    <t>POC15</t>
-  </si>
-  <si>
-    <t>POC16</t>
-  </si>
-  <si>
-    <t>POC17</t>
-  </si>
-  <si>
-    <t>POC18</t>
-  </si>
-  <si>
-    <t>POC19</t>
+    <t>Cap19-05X1</t>
+  </si>
+  <si>
+    <t>Cap19-05X2</t>
+  </si>
+  <si>
+    <t>Cap19-06X1</t>
+  </si>
+  <si>
+    <t>Cap19-06X2</t>
+  </si>
+  <si>
+    <t>Cap19-07X2</t>
+  </si>
+  <si>
+    <t>Cap19-08X1</t>
+  </si>
+  <si>
+    <t>Cap19-08X2</t>
+  </si>
+  <si>
+    <t>Cap19-12X1</t>
+  </si>
+  <si>
+    <t>Cap19-12X2</t>
+  </si>
+  <si>
+    <t>Cap19-17X1</t>
+  </si>
+  <si>
+    <t>Cap19-17X2</t>
+  </si>
+  <si>
+    <t>Cap19-18X1</t>
+  </si>
+  <si>
+    <t>Cap19-18X2</t>
+  </si>
+  <si>
+    <t>FG04_31_MI3</t>
+  </si>
+  <si>
+    <t>FG04_31_MI4 (1)</t>
+  </si>
+  <si>
+    <t>FG04_31_MI4</t>
   </si>
   <si>
     <t>POC20</t>
   </si>
   <si>
-    <t>POC21</t>
-  </si>
-  <si>
-    <t>POC22</t>
-  </si>
-  <si>
-    <t>POC23</t>
-  </si>
-  <si>
-    <t>POC24</t>
-  </si>
-  <si>
-    <t>POC25</t>
-  </si>
-  <si>
-    <t>POC26</t>
-  </si>
-  <si>
-    <t>POC27</t>
-  </si>
-  <si>
-    <t>POC28</t>
-  </si>
-  <si>
-    <t>POC29</t>
-  </si>
-  <si>
     <t>POC30</t>
   </si>
   <si>
@@ -181,7 +172,67 @@
     <t>POC34</t>
   </si>
   <si>
-    <t>POC9</t>
+    <t>POC35</t>
+  </si>
+  <si>
+    <t>POC36</t>
+  </si>
+  <si>
+    <t>POC37</t>
+  </si>
+  <si>
+    <t>POC38</t>
+  </si>
+  <si>
+    <t>POC39</t>
+  </si>
+  <si>
+    <t>POC40</t>
+  </si>
+  <si>
+    <t>POC41</t>
+  </si>
+  <si>
+    <t>POC42</t>
+  </si>
+  <si>
+    <t>POC43</t>
+  </si>
+  <si>
+    <t>POC44</t>
+  </si>
+  <si>
+    <t>POC45</t>
+  </si>
+  <si>
+    <t>POC47</t>
+  </si>
+  <si>
+    <t>POC48</t>
+  </si>
+  <si>
+    <t>POC49</t>
+  </si>
+  <si>
+    <t>POC50</t>
+  </si>
+  <si>
+    <t>POC51</t>
+  </si>
+  <si>
+    <t>POC52</t>
+  </si>
+  <si>
+    <t>POC53</t>
+  </si>
+  <si>
+    <t>POC55</t>
+  </si>
+  <si>
+    <t>POC56</t>
+  </si>
+  <si>
+    <t>POC57-0.04</t>
   </si>
   <si>
     <t>Flagged Warnings:</t>
@@ -542,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE27"/>
+  <dimension ref="A1:AE44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -648,88 +699,79 @@
         <v>30</v>
       </c>
       <c r="C2">
-        <v>104.3068688336057</v>
+        <v>102.8055901012403</v>
       </c>
       <c r="D2">
-        <v>1283.013374539996</v>
+        <v>1286.621100559627</v>
       </c>
       <c r="E2">
-        <v>3839.831365320886</v>
+        <v>224.6096138190325</v>
       </c>
       <c r="F2">
-        <v>1283.013224532496</v>
+        <v>1286.621150562127</v>
       </c>
       <c r="G2">
-        <v>11745.33809894446</v>
+        <v>336.6721688653458</v>
       </c>
       <c r="H2">
-        <v>1.134492608088072</v>
+        <v>0.6334872211494517</v>
       </c>
       <c r="I2">
-        <v>5.398439947593692</v>
+        <v>1.773255146888856</v>
       </c>
       <c r="J2">
-        <v>0.6678593964312827</v>
+        <v>0.3111781587925874</v>
       </c>
       <c r="K2">
-        <v>2.268985216176144</v>
+        <v>1.266974442298903</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M2">
-        <v>1387.320143368601</v>
+        <v>1389.426740663367</v>
       </c>
       <c r="N2">
-        <v>7636.849436568632</v>
+        <v>333.2923398851735</v>
       </c>
       <c r="O2">
-        <v>1387.320093366101</v>
+        <v>1389.426740663367</v>
       </c>
       <c r="P2">
-        <v>20282.4547100436</v>
+        <v>455.7211014185987</v>
       </c>
       <c r="Q2">
-        <v>0.9749725353934733</v>
+        <v>0.6092497250342414</v>
       </c>
       <c r="S2">
-        <v>6.474437443404418</v>
+        <v>1.908746463337239</v>
       </c>
       <c r="T2">
-        <v>0.6887684167855577</v>
+        <v>0.1594551035519094</v>
       </c>
       <c r="U2">
-        <v>1.949945070786947</v>
+        <v>1.218499450068483</v>
       </c>
       <c r="V2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W2">
-        <v>1262.944603045946</v>
+        <v>1266.277893539623</v>
       </c>
       <c r="X2">
-        <v>1700.72831878419</v>
+        <v>31.91457222355959</v>
       </c>
       <c r="Y2">
-        <v>2.899649728144492</v>
+        <v>0.5816256700254802</v>
       </c>
       <c r="Z2">
-        <v>1408.691199452309</v>
+        <v>1410.605407058006</v>
       </c>
       <c r="AA2">
-        <v>2082.545692040013</v>
+        <v>25.39522573493748</v>
       </c>
       <c r="AB2">
-        <v>2.11077329161178</v>
-      </c>
-      <c r="AC2">
-        <v>1369.669746083041</v>
-      </c>
-      <c r="AD2">
-        <v>261.6222194447227</v>
-      </c>
-      <c r="AE2">
-        <v>0.4861255031549175</v>
+        <v>0.5845863466799479</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -740,88 +782,79 @@
         <v>31</v>
       </c>
       <c r="C3">
-        <v>104.2516814865965</v>
+        <v>102.7595839649455</v>
       </c>
       <c r="D3">
-        <v>1283.137927604934</v>
+        <v>1286.620714031047</v>
       </c>
       <c r="E3">
-        <v>3178.549168244872</v>
+        <v>210.1796706631914</v>
       </c>
       <c r="F3">
-        <v>1283.137777597434</v>
+        <v>1286.620764033547</v>
       </c>
       <c r="G3">
-        <v>9814.731975612169</v>
+        <v>306.9724321930213</v>
       </c>
       <c r="H3">
-        <v>1.167504035745776</v>
+        <v>0.6383865448407688</v>
       </c>
       <c r="I3">
-        <v>4.753696008141983</v>
+        <v>2.07106898012511</v>
       </c>
       <c r="J3">
-        <v>0.6208175772282511</v>
+        <v>0.2160733409082576</v>
       </c>
       <c r="K3">
-        <v>2.335008071491553</v>
+        <v>1.276773089681538</v>
       </c>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M3">
-        <v>1387.38940908153</v>
+        <v>1389.380398000993</v>
       </c>
       <c r="N3">
-        <v>6469.823435608997</v>
+        <v>320.5674623731563</v>
       </c>
       <c r="O3">
-        <v>1387.38945908403</v>
+        <v>1389.380347998493</v>
       </c>
       <c r="P3">
-        <v>17127.54848611713</v>
+        <v>420.6360612248039</v>
       </c>
       <c r="Q3">
-        <v>0.9640872445658335</v>
+        <v>0.5988398242265743</v>
       </c>
       <c r="S3">
-        <v>5.292919625807597</v>
+        <v>2.765011827090027</v>
       </c>
       <c r="T3">
-        <v>0.7066241558540958</v>
+        <v>0.08817687940872126</v>
       </c>
       <c r="U3">
-        <v>1.928174489131667</v>
+        <v>1.197679648453149</v>
       </c>
       <c r="V3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W3">
-        <v>1263.099726006729</v>
+        <v>1266.32718377557</v>
       </c>
       <c r="X3">
-        <v>1378.427869524807</v>
+        <v>54.60760526554007</v>
       </c>
       <c r="Y3">
-        <v>2.76136804437558</v>
+        <v>1.039133994453138</v>
       </c>
       <c r="Z3">
-        <v>1408.758111614126</v>
+        <v>1410.647554620475</v>
       </c>
       <c r="AA3">
-        <v>1846.519084985494</v>
+        <v>35.78699831922494</v>
       </c>
       <c r="AB3">
-        <v>2.072105776566705</v>
-      </c>
-      <c r="AC3">
-        <v>1369.725665844658</v>
-      </c>
-      <c r="AD3">
-        <v>211.975747908649</v>
-      </c>
-      <c r="AE3">
-        <v>0.4808280785048223</v>
+        <v>0.2501892245700265</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -832,88 +865,88 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>104.1635370396491</v>
+        <v>102.9773754224191</v>
       </c>
       <c r="D4">
-        <v>1283.32126156703</v>
+        <v>1286.142237767746</v>
       </c>
       <c r="E4">
-        <v>4279.866495460506</v>
+        <v>920.4935290492161</v>
       </c>
       <c r="F4">
-        <v>1283.321411574531</v>
+        <v>1286.142287770246</v>
       </c>
       <c r="G4">
-        <v>13354.25524745115</v>
+        <v>1696.324883811872</v>
       </c>
       <c r="H4">
-        <v>1.188558274871424</v>
+        <v>0.7212904222261248</v>
       </c>
       <c r="I4">
-        <v>6.315370057949049</v>
+        <v>2.177302702733003</v>
       </c>
       <c r="J4">
-        <v>0.6004299056240009</v>
+        <v>0.5176053510957577</v>
       </c>
       <c r="K4">
-        <v>2.377116549742847</v>
+        <v>1.44258084445225</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M4">
-        <v>1387.48489861168</v>
+        <v>1389.119713195165</v>
       </c>
       <c r="N4">
-        <v>8736.961096970768</v>
+        <v>1508.364318263884</v>
       </c>
       <c r="O4">
-        <v>1387.48494861418</v>
+        <v>1389.119663192665</v>
       </c>
       <c r="P4">
-        <v>22921.02828497104</v>
+        <v>2443.250568463085</v>
       </c>
       <c r="Q4">
-        <v>0.967801889882731</v>
+        <v>0.6615841304737009</v>
       </c>
       <c r="S4">
-        <v>7.718528817855447</v>
+        <v>2.216104297512464</v>
       </c>
       <c r="T4">
-        <v>0.67586153306692</v>
+        <v>0.4049130720894457</v>
       </c>
       <c r="U4">
-        <v>1.935603779765462</v>
+        <v>1.323168260947402</v>
       </c>
       <c r="V4" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W4">
-        <v>1263.247068182799</v>
+        <v>1265.962243336075</v>
       </c>
       <c r="X4">
-        <v>1477.707005490268</v>
+        <v>175.2229714197016</v>
       </c>
       <c r="Y4">
-        <v>2.233651896878794</v>
+        <v>0.8996683702309629</v>
       </c>
       <c r="Z4">
-        <v>1408.862962359351</v>
+        <v>1410.403302997616</v>
       </c>
       <c r="AA4">
-        <v>2423.657579785595</v>
+        <v>214.0865936465165</v>
       </c>
       <c r="AB4">
-        <v>1.969957622305628</v>
+        <v>0.857111138550151</v>
       </c>
       <c r="AC4">
-        <v>1369.583496657191</v>
+        <v>1370.773465107819</v>
       </c>
       <c r="AD4">
-        <v>279.9988593827138</v>
+        <v>40.34983283573953</v>
       </c>
       <c r="AE4">
-        <v>0.4826647330738563</v>
+        <v>0.3306014445199942</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -924,88 +957,88 @@
         <v>33</v>
       </c>
       <c r="C5">
-        <v>104.1339592633685</v>
+        <v>102.9412109092927</v>
       </c>
       <c r="D5">
-        <v>1283.384592309311</v>
+        <v>1286.176034244954</v>
       </c>
       <c r="E5">
-        <v>4009.704418329633</v>
+        <v>1186.68533446968</v>
       </c>
       <c r="F5">
-        <v>1283.384742316812</v>
+        <v>1286.176084247454</v>
       </c>
       <c r="G5">
-        <v>12632.35276115954</v>
+        <v>2091.852275469249</v>
       </c>
       <c r="H5">
-        <v>1.197457599283966</v>
+        <v>0.7007096379405054</v>
       </c>
       <c r="I5">
-        <v>4.655257863802217</v>
+        <v>3.208730284702936</v>
       </c>
       <c r="J5">
-        <v>0.605324183956071</v>
+        <v>0.4773656411428394</v>
       </c>
       <c r="K5">
-        <v>2.394915198567932</v>
+        <v>1.401419275881011</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M5">
-        <v>1387.51865157768</v>
+        <v>1389.117345159247</v>
       </c>
       <c r="N5">
-        <v>8263.018665713696</v>
+        <v>1893.025453670518</v>
       </c>
       <c r="O5">
-        <v>1387.51870158018</v>
+        <v>1389.117295156747</v>
       </c>
       <c r="P5">
-        <v>21696.19596100426</v>
+        <v>2990.310283290652</v>
       </c>
       <c r="Q5">
-        <v>0.9701162088102482</v>
+        <v>0.6441009148779744</v>
       </c>
       <c r="S5">
-        <v>7.103503403951365</v>
+        <v>3.015289779798017</v>
       </c>
       <c r="T5">
-        <v>0.6718761717665203</v>
+        <v>0.4093867427770488</v>
       </c>
       <c r="U5">
-        <v>1.940232417620496</v>
+        <v>1.288201829755949</v>
       </c>
       <c r="V5" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W5">
-        <v>1263.38673308733</v>
+        <v>1265.893529941289</v>
       </c>
       <c r="X5">
-        <v>1451.41610076585</v>
+        <v>264.700248948888</v>
       </c>
       <c r="Y5">
-        <v>2.228220525021514</v>
+        <v>0.931200794818056</v>
       </c>
       <c r="Z5">
-        <v>1408.878688443767</v>
+        <v>1410.407101187656</v>
       </c>
       <c r="AA5">
-        <v>2293.099711384763</v>
+        <v>273.4821990473851</v>
       </c>
       <c r="AB5">
-        <v>1.955926425349598</v>
+        <v>0.7425755703095008</v>
       </c>
       <c r="AC5">
-        <v>1369.751575136229</v>
+        <v>1370.698349757371</v>
       </c>
       <c r="AD5">
-        <v>279.5638238955274</v>
+        <v>42.42996860646692</v>
       </c>
       <c r="AE5">
-        <v>0.483801754444614</v>
+        <v>0.3218661906255978</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -1016,88 +1049,79 @@
         <v>34</v>
       </c>
       <c r="C6">
-        <v>104.1082947488437</v>
+        <v>102.6857205703263</v>
       </c>
       <c r="D6">
-        <v>1283.442735932371</v>
+        <v>1286.703927391232</v>
       </c>
       <c r="E6">
-        <v>3719.098476323412</v>
+        <v>62.37462750994679</v>
       </c>
       <c r="F6">
-        <v>1283.442885939872</v>
+        <v>1286.703977393732</v>
       </c>
       <c r="G6">
-        <v>11838.63493853009</v>
+        <v>84.66974971734996</v>
       </c>
       <c r="H6">
-        <v>1.211477538793964</v>
+        <v>0.6376502519278551</v>
       </c>
       <c r="I6">
-        <v>4.358235721546903</v>
+        <v>2.034200738917988</v>
       </c>
       <c r="J6">
-        <v>0.6024606395818248</v>
+        <v>9.563345670926537E-10</v>
       </c>
       <c r="K6">
-        <v>2.422955077587928</v>
+        <v>1.27530050385571</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M6">
-        <v>1387.551130686215</v>
+        <v>1389.389747966559</v>
       </c>
       <c r="N6">
-        <v>7698.659148980008</v>
+        <v>96.18445065353157</v>
       </c>
       <c r="O6">
-        <v>1387.551180688715</v>
+        <v>1389.389697964059</v>
       </c>
       <c r="P6">
-        <v>20138.26694440611</v>
+        <v>124.5870733933524</v>
       </c>
       <c r="Q6">
-        <v>0.9669072085662109</v>
+        <v>0.6084233895789198</v>
       </c>
       <c r="S6">
-        <v>6.860069938740185</v>
+        <v>3.028424624954465</v>
       </c>
       <c r="T6">
-        <v>0.6705578738058641</v>
+        <v>4.406354603414542E-08</v>
       </c>
       <c r="U6">
-        <v>1.933814417132422</v>
+        <v>1.21684677915784</v>
       </c>
       <c r="V6" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W6">
-        <v>1263.405395905535</v>
+        <v>1266.029926728211</v>
       </c>
       <c r="X6">
-        <v>1346.410961338387</v>
+        <v>13.18824364577735</v>
       </c>
       <c r="Y6">
-        <v>2.173655308554195</v>
+        <v>0.3573772607201146</v>
       </c>
       <c r="Z6">
-        <v>1408.90890464617</v>
+        <v>1410.655709895359</v>
       </c>
       <c r="AA6">
-        <v>2178.64551880719</v>
+        <v>5.23923932664139</v>
       </c>
       <c r="AB6">
-        <v>1.970397762949396</v>
-      </c>
-      <c r="AC6">
-        <v>1369.746979108289</v>
-      </c>
-      <c r="AD6">
-        <v>250.6050942452976</v>
-      </c>
-      <c r="AE6">
-        <v>0.4822539161418356</v>
+        <v>0.2303438746642271</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -1108,88 +1132,70 @@
         <v>35</v>
       </c>
       <c r="C7">
-        <v>104.0682808896038</v>
+        <v>102.7989692201465</v>
       </c>
       <c r="D7">
-        <v>1283.528734209396</v>
+        <v>1286.53502393565</v>
       </c>
       <c r="E7">
-        <v>3487.196930249523</v>
+        <v>220.1082879845007</v>
       </c>
       <c r="F7">
-        <v>1283.528884216896</v>
+        <v>1286.53502393565</v>
       </c>
       <c r="G7">
-        <v>11081.9475229143</v>
+        <v>335.0522903012384</v>
       </c>
       <c r="H7">
-        <v>1.212772543554991</v>
+        <v>0.6557090885680108</v>
       </c>
       <c r="I7">
-        <v>3.788410498245351</v>
+        <v>1.605419310364716</v>
       </c>
       <c r="J7">
-        <v>0.5970576117838585</v>
+        <v>0.2651753055287928</v>
       </c>
       <c r="K7">
-        <v>2.425545087109982</v>
+        <v>1.311418177136022</v>
       </c>
       <c r="L7" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M7">
-        <v>1387.597115104</v>
+        <v>1389.334043158296</v>
       </c>
       <c r="N7">
-        <v>7159.69474071247</v>
+        <v>322.3923708054073</v>
       </c>
       <c r="O7">
-        <v>1387.5971651065</v>
+        <v>1389.333993155796</v>
       </c>
       <c r="P7">
-        <v>18582.6960670863</v>
+        <v>462.6359027527425</v>
       </c>
       <c r="Q7">
-        <v>0.96728708248518</v>
+        <v>0.6137593964709791</v>
       </c>
       <c r="S7">
-        <v>6.448742744967554</v>
+        <v>2.640248699723836</v>
       </c>
       <c r="T7">
-        <v>0.6513661834001512</v>
+        <v>0.2776791855301538</v>
       </c>
       <c r="U7">
-        <v>1.93457416497036</v>
+        <v>1.227518792941958</v>
       </c>
       <c r="V7" t="s">
-        <v>56</v>
-      </c>
-      <c r="W7">
-        <v>1263.469183664134</v>
-      </c>
-      <c r="X7">
-        <v>1264.070542778127</v>
-      </c>
-      <c r="Y7">
-        <v>2.183508439904035</v>
+        <v>73</v>
       </c>
       <c r="Z7">
-        <v>1408.986300998178</v>
+        <v>1410.617866490792</v>
       </c>
       <c r="AA7">
-        <v>2005.718413833568</v>
+        <v>51.51620535341678</v>
       </c>
       <c r="AB7">
-        <v>1.898713348399323</v>
-      </c>
-      <c r="AC7">
-        <v>1369.766982764778</v>
-      </c>
-      <c r="AD7">
-        <v>237.8244419584451</v>
-      </c>
-      <c r="AE7">
-        <v>0.4823750633957585</v>
+        <v>0.5977444346222675</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -1200,88 +1206,79 @@
         <v>36</v>
       </c>
       <c r="C8">
-        <v>104.0259695096818</v>
+        <v>102.7823504601445</v>
       </c>
       <c r="D8">
-        <v>1283.619989547175</v>
+        <v>1286.576910816088</v>
       </c>
       <c r="E8">
-        <v>3194.220878953314</v>
+        <v>212.8488592053265</v>
       </c>
       <c r="F8">
-        <v>1283.620139554675</v>
+        <v>1286.576960818588</v>
       </c>
       <c r="G8">
-        <v>10153.90453280614</v>
+        <v>321.7351137587453</v>
       </c>
       <c r="H8">
-        <v>1.227735768162747</v>
+        <v>0.6455928336963964</v>
       </c>
       <c r="I8">
-        <v>3.645389297906269</v>
+        <v>1.906798845116585</v>
       </c>
       <c r="J8">
-        <v>0.5656806680918467</v>
+        <v>0.2817290065074616</v>
       </c>
       <c r="K8">
-        <v>2.455471536325494</v>
+        <v>1.291185667392793</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M8">
-        <v>1387.646059061857</v>
+        <v>1389.359361281233</v>
       </c>
       <c r="N8">
-        <v>6590.460033205381</v>
+        <v>321.3192491184516</v>
       </c>
       <c r="O8">
-        <v>1387.646109064357</v>
+        <v>1389.359311278733</v>
       </c>
       <c r="P8">
-        <v>17064.38204512692</v>
+        <v>416.2995917885058</v>
       </c>
       <c r="Q8">
-        <v>0.969607859083025</v>
+        <v>0.6040574486625815</v>
       </c>
       <c r="S8">
-        <v>6.183825606847388</v>
+        <v>2.3721059152289</v>
       </c>
       <c r="T8">
-        <v>0.6389191173874661</v>
+        <v>0.02305499105589931</v>
       </c>
       <c r="U8">
-        <v>1.93921571816605</v>
+        <v>1.208114897325163</v>
       </c>
       <c r="V8" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W8">
-        <v>1263.554870044864</v>
+        <v>1266.266094080763</v>
       </c>
       <c r="X8">
-        <v>1130.568902193697</v>
+        <v>37.56328619961116</v>
       </c>
       <c r="Y8">
-        <v>2.096745821151021</v>
+        <v>0.6809942911908453</v>
       </c>
       <c r="Z8">
-        <v>1409.057086583224</v>
+        <v>1410.604997567064</v>
       </c>
       <c r="AA8">
-        <v>1798.712483155537</v>
+        <v>42.93297363697405</v>
       </c>
       <c r="AB8">
-        <v>1.818062820421157</v>
-      </c>
-      <c r="AC8">
-        <v>1369.81253067216</v>
-      </c>
-      <c r="AD8">
-        <v>206.0966054495482</v>
-      </c>
-      <c r="AE8">
-        <v>0.4834922279416978</v>
+        <v>0.2623544250622137</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -1292,88 +1289,88 @@
         <v>37</v>
       </c>
       <c r="C9">
-        <v>103.9621749398136</v>
+        <v>102.9754001653107</v>
       </c>
       <c r="D9">
-        <v>1283.770188777845</v>
+        <v>1286.103311953722</v>
       </c>
       <c r="E9">
-        <v>2936.784092252521</v>
+        <v>896.2525293153059</v>
       </c>
       <c r="F9">
-        <v>1283.770338785345</v>
+        <v>1286.103361956222</v>
       </c>
       <c r="G9">
-        <v>9339.470112043204</v>
+        <v>1639.448275493357</v>
       </c>
       <c r="H9">
-        <v>1.237343810776338</v>
+        <v>0.7329134660815226</v>
       </c>
       <c r="I9">
-        <v>2.854084204336967</v>
+        <v>2.028075381463807</v>
       </c>
       <c r="J9">
-        <v>0.5471433703801918</v>
+        <v>0.4564161196398066</v>
       </c>
       <c r="K9">
-        <v>2.474687621552676</v>
+        <v>1.465826932163045</v>
       </c>
       <c r="L9" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M9">
-        <v>1387.732163707658</v>
+        <v>1389.078812124033</v>
       </c>
       <c r="N9">
-        <v>6078.540568485294</v>
+        <v>1459.760978323083</v>
       </c>
       <c r="O9">
-        <v>1387.732513725159</v>
+        <v>1389.078762121533</v>
       </c>
       <c r="P9">
-        <v>15763.9771366546</v>
+        <v>2397.22305314877</v>
       </c>
       <c r="Q9">
-        <v>0.9670197974747295</v>
+        <v>0.6625529336299716</v>
       </c>
       <c r="S9">
-        <v>8.872289291089633</v>
+        <v>2.319941869706147</v>
       </c>
       <c r="T9">
-        <v>0.6462188370952329</v>
+        <v>0.4378093912022885</v>
       </c>
       <c r="U9">
-        <v>1.934039594949459</v>
+        <v>1.325105867259943</v>
       </c>
       <c r="V9" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W9">
-        <v>1263.720374410581</v>
+        <v>1265.877696220473</v>
       </c>
       <c r="X9">
-        <v>1037.863808223503</v>
+        <v>171.417465956339</v>
       </c>
       <c r="Y9">
-        <v>2.065022438449267</v>
+        <v>0.9313901191944396</v>
       </c>
       <c r="Z9">
-        <v>1409.125072208905</v>
+        <v>1410.363059304737</v>
       </c>
       <c r="AA9">
-        <v>1795.574782926477</v>
+        <v>212.9871538672664</v>
       </c>
       <c r="AB9">
-        <v>1.877440788141546</v>
+        <v>0.7876349515453347</v>
       </c>
       <c r="AC9">
-        <v>1370.051139767008</v>
+        <v>1372.237604945571</v>
       </c>
       <c r="AD9">
-        <v>238.9778138209251</v>
+        <v>13.83244241589734</v>
       </c>
       <c r="AE9">
-        <v>0.482276060531027</v>
+        <v>0.3310915476547392</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -1384,88 +1381,88 @@
         <v>38</v>
       </c>
       <c r="C10">
-        <v>103.8722401618988</v>
+        <v>102.94708644246</v>
       </c>
       <c r="D10">
-        <v>1283.955803452305</v>
+        <v>1286.145918503546</v>
       </c>
       <c r="E10">
-        <v>2388.276648167718</v>
+        <v>533.172656219509</v>
       </c>
       <c r="F10">
-        <v>1283.955953459806</v>
+        <v>1286.145968506046</v>
       </c>
       <c r="G10">
-        <v>7618.773987539793</v>
+        <v>952.3493264403465</v>
       </c>
       <c r="H10">
-        <v>1.245533492548427</v>
+        <v>0.7296832127206719</v>
       </c>
       <c r="I10">
-        <v>2.761448738475937</v>
+        <v>1.975340396997963</v>
       </c>
       <c r="J10">
-        <v>0.5387053518477318</v>
+        <v>0.4045161318849489</v>
       </c>
       <c r="K10">
-        <v>2.491066985096854</v>
+        <v>1.459366425441344</v>
       </c>
       <c r="L10" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M10">
-        <v>1387.828143619204</v>
+        <v>1389.093004946006</v>
       </c>
       <c r="N10">
-        <v>4951.057849112833</v>
+        <v>879.2090301095086</v>
       </c>
       <c r="O10">
-        <v>1387.828193621704</v>
+        <v>1389.093054948506</v>
       </c>
       <c r="P10">
-        <v>12641.1392659416</v>
+        <v>1391.42140976273</v>
       </c>
       <c r="Q10">
-        <v>0.9625193148172664</v>
+        <v>0.6449012161936417</v>
       </c>
       <c r="S10">
-        <v>4.971584073179956</v>
+        <v>2.11650108716624</v>
       </c>
       <c r="T10">
-        <v>0.6223735573184662</v>
+        <v>0.4109728342957012</v>
       </c>
       <c r="U10">
-        <v>1.925038629634533</v>
+        <v>1.289802432387283</v>
       </c>
       <c r="V10" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W10">
-        <v>1263.951743402573</v>
+        <v>1265.889710642899</v>
       </c>
       <c r="X10">
-        <v>836.4825970663769</v>
+        <v>96.08181720000948</v>
       </c>
       <c r="Y10">
-        <v>2.00342119712677</v>
+        <v>0.7311990739659359</v>
       </c>
       <c r="Z10">
-        <v>1409.223254165374</v>
+        <v>1410.415886266758</v>
       </c>
       <c r="AA10">
-        <v>1317.927638114184</v>
+        <v>104.9420730653179</v>
       </c>
       <c r="AB10">
-        <v>1.620029948384114</v>
+        <v>0.7494426558302814</v>
       </c>
       <c r="AC10">
-        <v>1370.048410299656</v>
+        <v>1370.799601392132</v>
       </c>
       <c r="AD10">
-        <v>150.2337829067039</v>
+        <v>21.84401953284096</v>
       </c>
       <c r="AE10">
-        <v>0.4796569127462339</v>
+        <v>0.3222924041377855</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -1476,88 +1473,70 @@
         <v>39</v>
       </c>
       <c r="C11">
-        <v>103.7654814210073</v>
+        <v>102.8160045057161</v>
       </c>
       <c r="D11">
-        <v>1284.202532075621</v>
+        <v>1286.343355190082</v>
       </c>
       <c r="E11">
-        <v>2090.673940178109</v>
+        <v>242.2540204113231</v>
       </c>
       <c r="F11">
-        <v>1284.202682083122</v>
+        <v>1286.343355190082</v>
       </c>
       <c r="G11">
-        <v>6546.65680333308</v>
+        <v>375.2031988555228</v>
       </c>
       <c r="H11">
-        <v>1.232513511188887</v>
+        <v>0.6845415678658096</v>
       </c>
       <c r="I11">
-        <v>3.165116909802714</v>
+        <v>2.049196104130471</v>
       </c>
       <c r="J11">
-        <v>0.5163801204498372</v>
+        <v>0.185655760595126</v>
       </c>
       <c r="K11">
-        <v>2.465027022377773</v>
+        <v>1.369083135731619</v>
       </c>
       <c r="L11" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M11">
-        <v>1387.968113501629</v>
+        <v>1389.159359695798</v>
       </c>
       <c r="N11">
-        <v>4288.929722369199</v>
+        <v>366.7872653256723</v>
       </c>
       <c r="O11">
-        <v>1387.968163504129</v>
+        <v>1389.159359695798</v>
       </c>
       <c r="P11">
-        <v>10734.29045164146</v>
+        <v>517.813161254204</v>
       </c>
       <c r="Q11">
-        <v>0.948608219047877</v>
+        <v>0.6186177539891247</v>
       </c>
       <c r="S11">
-        <v>5.084164877647385</v>
+        <v>2.238120182394155</v>
       </c>
       <c r="T11">
-        <v>0.6078546766944218</v>
+        <v>0.2082280263245472</v>
       </c>
       <c r="U11">
-        <v>1.897216438095754</v>
+        <v>1.237235507978249</v>
       </c>
       <c r="V11" t="s">
-        <v>56</v>
-      </c>
-      <c r="W11">
-        <v>1264.168775073954</v>
-      </c>
-      <c r="X11">
-        <v>709.161146145618</v>
-      </c>
-      <c r="Y11">
-        <v>1.804919588073626</v>
+        <v>73</v>
       </c>
       <c r="Z11">
-        <v>1409.400390401279</v>
+        <v>1410.387239083391</v>
       </c>
       <c r="AA11">
-        <v>1140.560586485238</v>
+        <v>32.07731699632706</v>
       </c>
       <c r="AB11">
-        <v>1.54157979140134</v>
-      </c>
-      <c r="AC11">
-        <v>1370.135865115825</v>
-      </c>
-      <c r="AD11">
-        <v>144.9272182675785</v>
-      </c>
-      <c r="AE11">
-        <v>0.4729121979550922</v>
+        <v>0.6432420957908963</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -1568,88 +1547,79 @@
         <v>40</v>
       </c>
       <c r="C12">
-        <v>103.6687175154179</v>
+        <v>102.8253919308345</v>
       </c>
       <c r="D12">
-        <v>1284.419138792759</v>
+        <v>1286.497264960275</v>
       </c>
       <c r="E12">
-        <v>1864.65988520681</v>
+        <v>445.324622060049</v>
       </c>
       <c r="F12">
-        <v>1284.419288800259</v>
+        <v>1286.497314962775</v>
       </c>
       <c r="G12">
-        <v>5681.16132264406</v>
+        <v>691.9154047771509</v>
       </c>
       <c r="H12">
-        <v>1.20749454522914</v>
+        <v>0.6637934262873955</v>
       </c>
       <c r="I12">
-        <v>3.077314001349746</v>
+        <v>2.538444738068544</v>
       </c>
       <c r="J12">
-        <v>0.5011770176148037</v>
+        <v>0.2808893026814239</v>
       </c>
       <c r="K12">
-        <v>2.41498909045828</v>
+        <v>1.327586852574791</v>
       </c>
       <c r="L12" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M12">
-        <v>1388.087956313177</v>
+        <v>1389.322706893609</v>
       </c>
       <c r="N12">
-        <v>3825.840690857817</v>
+        <v>680.6616800239143</v>
       </c>
       <c r="O12">
-        <v>1388.088006315677</v>
+        <v>1389.322706893609</v>
       </c>
       <c r="P12">
-        <v>9288.064503910058</v>
+        <v>974.7596103809302</v>
       </c>
       <c r="Q12">
-        <v>0.927544445000744</v>
+        <v>0.6175270437300351</v>
       </c>
       <c r="S12">
-        <v>4.655614574408858</v>
+        <v>2.730379802719991</v>
       </c>
       <c r="T12">
-        <v>0.5883458216353071</v>
+        <v>0.2543294860763184</v>
       </c>
       <c r="U12">
-        <v>1.855088890001488</v>
+        <v>1.23505408746007</v>
       </c>
       <c r="V12" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W12">
-        <v>1264.350139846816</v>
+        <v>1266.257849753662</v>
       </c>
       <c r="X12">
-        <v>633.7166162991255</v>
+        <v>79.1674627595747</v>
       </c>
       <c r="Y12">
-        <v>1.689111056598466</v>
+        <v>0.7281188015104286</v>
       </c>
       <c r="Z12">
-        <v>1409.474536216039</v>
+        <v>1410.524958902432</v>
       </c>
       <c r="AA12">
-        <v>985.2028685074564</v>
+        <v>74.31309649497031</v>
       </c>
       <c r="AB12">
-        <v>1.483104553620565</v>
-      </c>
-      <c r="AC12">
-        <v>1370.16718049111</v>
-      </c>
-      <c r="AD12">
-        <v>119.0540091913976</v>
-      </c>
-      <c r="AE12">
-        <v>0.4625597675038267</v>
+        <v>0.6252962692255352</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -1660,88 +1630,88 @@
         <v>41</v>
       </c>
       <c r="C13">
-        <v>103.6035942196334</v>
+        <v>102.8840062830866</v>
       </c>
       <c r="D13">
-        <v>1284.568802657673</v>
+        <v>1286.211853439394</v>
       </c>
       <c r="E13">
-        <v>2586.692332607533</v>
+        <v>670.6702135383302</v>
       </c>
       <c r="F13">
-        <v>1284.568852660173</v>
+        <v>1286.211903441894</v>
       </c>
       <c r="G13">
-        <v>7704.446690529956</v>
+        <v>1112.210981814327</v>
       </c>
       <c r="H13">
-        <v>1.160084543789299</v>
+        <v>0.6717629914590478</v>
       </c>
       <c r="I13">
-        <v>4.948626783029892</v>
+        <v>2.189009763643276</v>
       </c>
       <c r="J13">
-        <v>0.5415643698910166</v>
+        <v>0.4272422869722132</v>
       </c>
       <c r="K13">
-        <v>2.320169087578598</v>
+        <v>1.343525982918096</v>
       </c>
       <c r="L13" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M13">
-        <v>1388.171496832304</v>
+        <v>1389.095959727481</v>
       </c>
       <c r="N13">
-        <v>5246.597702313864</v>
+        <v>1052.607753339384</v>
       </c>
       <c r="O13">
-        <v>1388.172446879806</v>
+        <v>1389.095909724981</v>
       </c>
       <c r="P13">
-        <v>12381.65477078189</v>
+        <v>1591.60312845536</v>
       </c>
       <c r="Q13">
-        <v>0.9031822393585274</v>
+        <v>0.6297502783821755</v>
       </c>
       <c r="S13">
-        <v>9.271364044695853</v>
+        <v>2.162337831445108</v>
       </c>
       <c r="T13">
-        <v>0.5909832075601144</v>
+        <v>0.3516788186107476</v>
       </c>
       <c r="U13">
-        <v>1.806364478717055</v>
+        <v>1.259500556764351</v>
       </c>
       <c r="V13" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W13">
-        <v>1264.471077668715</v>
+        <v>1265.996703737489</v>
       </c>
       <c r="X13">
-        <v>882.490173254227</v>
+        <v>117.7053251983629</v>
       </c>
       <c r="Y13">
-        <v>1.743716688909511</v>
+        <v>0.8482680706879058</v>
       </c>
       <c r="Z13">
-        <v>1409.554369581117</v>
+        <v>1410.374899704</v>
       </c>
       <c r="AA13">
-        <v>1374.562471119839</v>
+        <v>128.7119747216973</v>
       </c>
       <c r="AB13">
-        <v>1.422706981629337</v>
+        <v>0.7088913097795355</v>
       </c>
       <c r="AC13">
-        <v>1370.175236972745</v>
+        <v>1370.764016232836</v>
       </c>
       <c r="AD13">
-        <v>210.668805240445</v>
+        <v>22.90470474259168</v>
       </c>
       <c r="AE13">
-        <v>0.4518965137750903</v>
+        <v>0.3146994480177396</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -1752,88 +1722,88 @@
         <v>42</v>
       </c>
       <c r="C14">
-        <v>103.5465391138425</v>
+        <v>102.8796708835193</v>
       </c>
       <c r="D14">
-        <v>1284.689867693646</v>
+        <v>1286.384827385504</v>
       </c>
       <c r="E14">
-        <v>2482.91092042634</v>
+        <v>698.6657921298926</v>
       </c>
       <c r="F14">
-        <v>1284.689917696146</v>
+        <v>1286.384877388004</v>
       </c>
       <c r="G14">
-        <v>7243.683721574982</v>
+        <v>1132.088823741904</v>
       </c>
       <c r="H14">
-        <v>1.124051134416373</v>
+        <v>0.6736757539522844</v>
       </c>
       <c r="I14">
-        <v>4.985321659503223</v>
+        <v>3.323839703071039</v>
       </c>
       <c r="J14">
-        <v>0.5652992560425192</v>
+        <v>0.3567166449089828</v>
       </c>
       <c r="K14">
-        <v>2.248102268832746</v>
+        <v>1.347351507904569</v>
       </c>
       <c r="L14" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M14">
-        <v>1388.236406807488</v>
+        <v>1389.264498269024</v>
       </c>
       <c r="N14">
-        <v>4936.992189492417</v>
+        <v>1084.440788544693</v>
       </c>
       <c r="O14">
-        <v>1388.236456809988</v>
+        <v>1389.264548271524</v>
       </c>
       <c r="P14">
-        <v>11475.97157623405</v>
+        <v>1603.545036782327</v>
       </c>
       <c r="Q14">
-        <v>0.887099567228144</v>
+        <v>0.6243292176462568</v>
       </c>
       <c r="S14">
-        <v>6.630220352823651</v>
+        <v>3.392558022865032</v>
       </c>
       <c r="T14">
-        <v>0.5899178618240037</v>
+        <v>0.3137273444228676</v>
       </c>
       <c r="U14">
-        <v>1.774199134456288</v>
+        <v>1.248658435292514</v>
       </c>
       <c r="V14" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W14">
-        <v>1264.58734847381</v>
+        <v>1266.153692188911</v>
       </c>
       <c r="X14">
-        <v>805.5720385284033</v>
+        <v>141.0650177100912</v>
       </c>
       <c r="Y14">
-        <v>1.663329243442161</v>
+        <v>0.8176373505864143</v>
       </c>
       <c r="Z14">
-        <v>1409.62558289162</v>
+        <v>1410.54228421546</v>
       </c>
       <c r="AA14">
-        <v>1198.225753970435</v>
+        <v>126.8239989280499</v>
       </c>
       <c r="AB14">
-        <v>1.34341137011503</v>
+        <v>0.7071057794193715</v>
       </c>
       <c r="AC14">
-        <v>1370.217793810498</v>
+        <v>1370.833574014715</v>
       </c>
       <c r="AD14">
-        <v>150.2887439722509</v>
+        <v>19.49627388428174</v>
       </c>
       <c r="AE14">
-        <v>0.4421306741921666</v>
+        <v>0.3119337522525792</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -1844,88 +1814,88 @@
         <v>43</v>
       </c>
       <c r="C15">
-        <v>103.5071373727187</v>
+        <v>103.2407789628148</v>
       </c>
       <c r="D15">
-        <v>1284.813769410711</v>
+        <v>1285.256509927521</v>
       </c>
       <c r="E15">
-        <v>2388.376248595952</v>
+        <v>1317.567897091061</v>
       </c>
       <c r="F15">
-        <v>1284.813819413211</v>
+        <v>1285.256559930021</v>
       </c>
       <c r="G15">
-        <v>6732.445233220186</v>
+        <v>3642.828182553853</v>
       </c>
       <c r="H15">
-        <v>1.106204202839708</v>
+        <v>1.069511451766251</v>
       </c>
       <c r="I15">
-        <v>4.788724724238969</v>
+        <v>5.158494024396302</v>
       </c>
       <c r="J15">
-        <v>0.5255773702872207</v>
+        <v>0.5487401777822166</v>
       </c>
       <c r="K15">
-        <v>2.212408405679417</v>
+        <v>2.139022903532502</v>
       </c>
       <c r="L15" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M15">
-        <v>1388.320006738428</v>
+        <v>1388.497388895336</v>
       </c>
       <c r="N15">
-        <v>4772.777422846685</v>
+        <v>2608.508794280448</v>
       </c>
       <c r="O15">
-        <v>1388.32095678593</v>
+        <v>1388.497338892836</v>
       </c>
       <c r="P15">
-        <v>10690.84943213231</v>
+        <v>5656.614950503998</v>
       </c>
       <c r="Q15">
-        <v>0.8614204578183269</v>
+        <v>0.8351215894799744</v>
       </c>
       <c r="S15">
-        <v>9.0239629527163</v>
+        <v>4.669884374432447</v>
       </c>
       <c r="T15">
-        <v>0.5809975619034004</v>
+        <v>0.559311370808566</v>
       </c>
       <c r="U15">
-        <v>1.722840915636654</v>
+        <v>1.670243178959949</v>
       </c>
       <c r="V15" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W15">
-        <v>1264.73290304539</v>
+        <v>1265.210439478499</v>
       </c>
       <c r="X15">
-        <v>736.4121735844601</v>
+        <v>598.5711363221146</v>
       </c>
       <c r="Y15">
-        <v>1.531437462050061</v>
+        <v>1.408294045131258</v>
       </c>
       <c r="Z15">
-        <v>1409.680149577843</v>
+        <v>1409.877548021207</v>
       </c>
       <c r="AA15">
-        <v>1190.818332325692</v>
+        <v>776.2535829118409</v>
       </c>
       <c r="AB15">
-        <v>1.323385024733842</v>
+        <v>1.016252065828917</v>
       </c>
       <c r="AC15">
-        <v>1370.217617865803</v>
+        <v>1370.299587139649</v>
       </c>
       <c r="AD15">
-        <v>187.6957963140682</v>
+        <v>81.40218736009649</v>
       </c>
       <c r="AE15">
-        <v>0.4308785816634384</v>
+        <v>0.4168529878842909</v>
       </c>
     </row>
     <row r="16" spans="1:31">
@@ -1936,88 +1906,88 @@
         <v>44</v>
       </c>
       <c r="C16">
-        <v>103.4549982454412</v>
+        <v>103.7097002729488</v>
       </c>
       <c r="D16">
-        <v>1284.906047597995</v>
+        <v>1284.338696958891</v>
       </c>
       <c r="E16">
-        <v>2315.769272627398</v>
+        <v>922.5386585998286</v>
       </c>
       <c r="F16">
-        <v>1284.906097600495</v>
+        <v>1284.338746961392</v>
       </c>
       <c r="G16">
-        <v>6396.346473542497</v>
+        <v>2796.777526798034</v>
       </c>
       <c r="H16">
-        <v>1.069313542549715</v>
+        <v>1.148573786268707</v>
       </c>
       <c r="I16">
-        <v>4.554494124998676</v>
+        <v>2.149885912257316</v>
       </c>
       <c r="J16">
-        <v>0.5532987249721325</v>
+        <v>0.6017565817752606</v>
       </c>
       <c r="K16">
-        <v>2.138627085099431</v>
+        <v>2.297147572537414</v>
       </c>
       <c r="L16" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M16">
-        <v>1388.361045843436</v>
+        <v>1388.04849723684</v>
       </c>
       <c r="N16">
-        <v>4556.621297157805</v>
+        <v>1857.680674395034</v>
       </c>
       <c r="O16">
-        <v>1388.361095845936</v>
+        <v>1388.04844723434</v>
       </c>
       <c r="P16">
-        <v>10112.6625551637</v>
+        <v>4581.008336356091</v>
       </c>
       <c r="Q16">
-        <v>0.8483652862146112</v>
+        <v>0.9140380482629511</v>
       </c>
       <c r="S16">
-        <v>5.884054684406574</v>
+        <v>3.51007572705472</v>
       </c>
       <c r="T16">
-        <v>0.5841540760044309</v>
+        <v>0.6550531493954189</v>
       </c>
       <c r="U16">
-        <v>1.696730572429222</v>
+        <v>1.828076096525902</v>
       </c>
       <c r="V16" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W16">
-        <v>1264.76748518432</v>
+        <v>1264.206578465222</v>
       </c>
       <c r="X16">
-        <v>698.5236452194148</v>
+        <v>396.2028359606486</v>
       </c>
       <c r="Y16">
-        <v>1.520650598145397</v>
+        <v>2.043774649113944</v>
       </c>
       <c r="Z16">
-        <v>1409.747046965419</v>
+        <v>1409.417092486725</v>
       </c>
       <c r="AA16">
-        <v>1032.692635542177</v>
+        <v>533.4528367985273</v>
       </c>
       <c r="AB16">
-        <v>1.227500414353929</v>
+        <v>1.558370024014355</v>
       </c>
       <c r="AC16">
-        <v>1370.25927778879</v>
+        <v>1370.217090411967</v>
       </c>
       <c r="AD16">
-        <v>135.7604129024586</v>
+        <v>64.48343335693143</v>
       </c>
       <c r="AE16">
-        <v>0.4228657339033727</v>
+        <v>0.4562893454226851</v>
       </c>
     </row>
     <row r="17" spans="1:31">
@@ -2028,88 +1998,88 @@
         <v>45</v>
       </c>
       <c r="C17">
-        <v>103.4267483836068</v>
+        <v>103.4175291494134</v>
       </c>
       <c r="D17">
-        <v>1284.981394358522</v>
+        <v>1284.88437560771</v>
       </c>
       <c r="E17">
-        <v>2300.273595644966</v>
+        <v>548.8726202930238</v>
       </c>
       <c r="F17">
-        <v>1284.982044391024</v>
+        <v>1284.88442561021</v>
       </c>
       <c r="G17">
-        <v>6202.138685970984</v>
+        <v>1568.7336708113</v>
       </c>
       <c r="H17">
-        <v>1.033023981112026</v>
+        <v>1.079868050458035</v>
       </c>
       <c r="I17">
-        <v>5.482938291244799</v>
+        <v>2.266708483424015</v>
       </c>
       <c r="J17">
-        <v>0.5850772675955311</v>
+        <v>0.6081938480905886</v>
       </c>
       <c r="K17">
-        <v>2.066047962224053</v>
+        <v>2.159736100916069</v>
       </c>
       <c r="L17" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M17">
-        <v>1388.408042737129</v>
+        <v>1388.302004762123</v>
       </c>
       <c r="N17">
-        <v>4434.804275450179</v>
+        <v>1108.085737767967</v>
       </c>
       <c r="O17">
-        <v>1388.408792774631</v>
+        <v>1388.301954759623</v>
       </c>
       <c r="P17">
-        <v>9613.33883976337</v>
+        <v>2484.730488673055</v>
       </c>
       <c r="Q17">
-        <v>0.8351110766917861</v>
+        <v>0.8460219514377698</v>
       </c>
       <c r="S17">
-        <v>6.151251014232501</v>
+        <v>2.602541681256802</v>
       </c>
       <c r="T17">
-        <v>0.5743016085467961</v>
+        <v>0.6109728170554275</v>
       </c>
       <c r="U17">
-        <v>1.670222153383572</v>
+        <v>1.69204390287554</v>
       </c>
       <c r="V17" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W17">
-        <v>1264.820592855419</v>
+        <v>1264.775134994546</v>
       </c>
       <c r="X17">
-        <v>775.4600106271969</v>
+        <v>205.7724520937339</v>
       </c>
       <c r="Y17">
-        <v>1.673953685658865</v>
+        <v>1.755715889197963</v>
       </c>
       <c r="Z17">
-        <v>1409.784045893438</v>
+        <v>1409.711828666435</v>
       </c>
       <c r="AA17">
-        <v>1049.402882333457</v>
+        <v>253.8787288805055</v>
       </c>
       <c r="AB17">
-        <v>1.228510759712377</v>
+        <v>1.214023445807388</v>
       </c>
       <c r="AC17">
-        <v>1370.258125195695</v>
+        <v>1370.262688042509</v>
       </c>
       <c r="AD17">
-        <v>152.320885660391</v>
+        <v>40.6288800707526</v>
       </c>
       <c r="AE17">
-        <v>0.4177857397660348</v>
+        <v>0.4223311393061437</v>
       </c>
     </row>
     <row r="18" spans="1:31">
@@ -2120,88 +2090,88 @@
         <v>46</v>
       </c>
       <c r="C18">
-        <v>103.3926807259272</v>
+        <v>103.6683491378933</v>
       </c>
       <c r="D18">
-        <v>1285.062034510263</v>
+        <v>1284.419463179161</v>
       </c>
       <c r="E18">
-        <v>2323.127372529151</v>
+        <v>1872.824979173804</v>
       </c>
       <c r="F18">
-        <v>1285.062884552765</v>
+        <v>1284.419513181661</v>
       </c>
       <c r="G18">
-        <v>6057.890402897044</v>
+        <v>5888.652364238065</v>
       </c>
       <c r="H18">
-        <v>0.9972625794394876</v>
+        <v>1.20499410646136</v>
       </c>
       <c r="I18">
-        <v>5.730086524327763</v>
+        <v>5.457489859259095</v>
       </c>
       <c r="J18">
-        <v>0.5914877436995563</v>
+        <v>0.5732545632932544</v>
       </c>
       <c r="K18">
-        <v>1.994525158878975</v>
+        <v>2.409988212922721</v>
       </c>
       <c r="L18" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M18">
-        <v>1388.454915246191</v>
+        <v>1388.087912322055</v>
       </c>
       <c r="N18">
-        <v>4438.371926890079</v>
+        <v>3833.362037325242</v>
       </c>
       <c r="O18">
-        <v>1388.455565278692</v>
+        <v>1388.087862319555</v>
       </c>
       <c r="P18">
-        <v>9365.639092298843</v>
+        <v>9475.143447923992</v>
       </c>
       <c r="Q18">
-        <v>0.8103405583542487</v>
+        <v>0.9265980911721829</v>
       </c>
       <c r="S18">
-        <v>6.94649156131828</v>
+        <v>7.085669141949456</v>
       </c>
       <c r="T18">
-        <v>0.5804528465650867</v>
+        <v>0.6271876553598784</v>
       </c>
       <c r="U18">
-        <v>1.620681116708497</v>
+        <v>1.853196182344366</v>
       </c>
       <c r="V18" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W18">
-        <v>1264.969098499307</v>
+        <v>1264.344208843684</v>
       </c>
       <c r="X18">
-        <v>784.8783409700975</v>
+        <v>860.649600069093</v>
       </c>
       <c r="Y18">
-        <v>1.667706573275931</v>
+        <v>2.27944567522512</v>
       </c>
       <c r="Z18">
-        <v>1409.838595646424</v>
+        <v>1409.45913652981</v>
       </c>
       <c r="AA18">
-        <v>1042.243576708711</v>
+        <v>1057.630503233597</v>
       </c>
       <c r="AB18">
-        <v>1.185756455498557</v>
+        <v>1.556849963286087</v>
       </c>
       <c r="AC18">
-        <v>1370.276920845476</v>
+        <v>1370.169387196477</v>
       </c>
       <c r="AD18">
-        <v>146.6329943895221</v>
+        <v>123.6354714394227</v>
       </c>
       <c r="AE18">
-        <v>0.4053822887395697</v>
+        <v>0.4625590464215648</v>
       </c>
     </row>
     <row r="19" spans="1:31">
@@ -2212,88 +2182,88 @@
         <v>47</v>
       </c>
       <c r="C19">
-        <v>103.3631881470931</v>
+        <v>103.1252710007964</v>
       </c>
       <c r="D19">
-        <v>1285.123179675461</v>
+        <v>1285.703612812319</v>
       </c>
       <c r="E19">
-        <v>2581.190778777873</v>
+        <v>2058.914446166538</v>
       </c>
       <c r="F19">
-        <v>1285.123729702963</v>
+        <v>1285.703662814819</v>
       </c>
       <c r="G19">
-        <v>6641.465948277015</v>
+        <v>4389.94916687396</v>
       </c>
       <c r="H19">
-        <v>0.9855144175296043</v>
+        <v>0.8204531236309602</v>
       </c>
       <c r="I19">
-        <v>6.577885916676368</v>
+        <v>3.88211220351241</v>
       </c>
       <c r="J19">
-        <v>0.5829147532034773</v>
+        <v>0.5614815952571084</v>
       </c>
       <c r="K19">
-        <v>1.971028835059209</v>
+        <v>1.64090624726192</v>
       </c>
       <c r="L19" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M19">
-        <v>1388.486967852556</v>
+        <v>1388.828983818116</v>
       </c>
       <c r="N19">
-        <v>4874.70196471591</v>
+        <v>3709.397285165281</v>
       </c>
       <c r="O19">
-        <v>1388.486917850056</v>
+        <v>1388.828933815616</v>
       </c>
       <c r="P19">
-        <v>10229.41831975356</v>
+        <v>6753.127586608442</v>
       </c>
       <c r="Q19">
-        <v>0.8114367885265161</v>
+        <v>0.7108223001286644</v>
       </c>
       <c r="S19">
-        <v>8.765424504902491</v>
+        <v>3.594078650043697</v>
       </c>
       <c r="T19">
-        <v>0.5605238237831689</v>
+        <v>0.5238295006657628</v>
       </c>
       <c r="U19">
-        <v>1.622873577053032</v>
+        <v>1.421644600257329</v>
       </c>
       <c r="V19" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W19">
-        <v>1265.005505290838</v>
+        <v>1265.546910585514</v>
       </c>
       <c r="X19">
-        <v>851.5505370432209</v>
+        <v>528.8301167980744</v>
       </c>
       <c r="Y19">
-        <v>1.612441536179605</v>
+        <v>1.197405866578045</v>
       </c>
       <c r="Z19">
-        <v>1409.843363583897</v>
+        <v>1410.087549852962</v>
       </c>
       <c r="AA19">
-        <v>876.396401165109</v>
+        <v>672.1564012123152</v>
       </c>
       <c r="AB19">
-        <v>1.122670340990837</v>
+        <v>0.8699190533038033</v>
       </c>
       <c r="AC19">
-        <v>1370.296690366602</v>
+        <v>1370.675824270695</v>
       </c>
       <c r="AD19">
-        <v>140.1272006353673</v>
+        <v>91.02463635997363</v>
       </c>
       <c r="AE19">
-        <v>0.4044235461211767</v>
+        <v>0.3549347311165698</v>
       </c>
     </row>
     <row r="20" spans="1:31">
@@ -2304,88 +2274,88 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>103.2706243286584</v>
+        <v>103.0190212922732</v>
       </c>
       <c r="D20">
-        <v>1285.368110127883</v>
+        <v>1285.956360530768</v>
       </c>
       <c r="E20">
-        <v>2444.921132100177</v>
+        <v>7081.384296017904</v>
       </c>
       <c r="F20">
-        <v>1285.368160130383</v>
+        <v>1285.956410533268</v>
       </c>
       <c r="G20">
-        <v>5771.986350431068</v>
+        <v>13792.9221712317</v>
       </c>
       <c r="H20">
-        <v>0.909979164652263</v>
+        <v>0.7649369026717137</v>
       </c>
       <c r="I20">
-        <v>4.347486771026699</v>
+        <v>11.69522568738774</v>
       </c>
       <c r="J20">
-        <v>0.5646184572825417</v>
+        <v>0.508987342377775</v>
       </c>
       <c r="K20">
-        <v>1.819958329304526</v>
+        <v>1.529873805343427</v>
       </c>
       <c r="L20" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M20">
-        <v>1388.638734456541</v>
+        <v>1388.975481828041</v>
       </c>
       <c r="N20">
-        <v>4532.217356622721</v>
+        <v>12155.24090405866</v>
       </c>
       <c r="O20">
-        <v>1388.638784459042</v>
+        <v>1388.975431825541</v>
       </c>
       <c r="P20">
-        <v>8941.326521255594</v>
+        <v>20704.06767165739</v>
       </c>
       <c r="Q20">
-        <v>0.7612526120843974</v>
+        <v>0.6792926605571197</v>
       </c>
       <c r="S20">
-        <v>4.622959579113912</v>
+        <v>11.71076322722051</v>
       </c>
       <c r="T20">
-        <v>0.5572909081190081</v>
+        <v>0.4685782164197362</v>
       </c>
       <c r="U20">
-        <v>1.522505224168795</v>
+        <v>1.358585321114239</v>
       </c>
       <c r="V20" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W20">
-        <v>1265.246950237366</v>
+        <v>1265.749870596261</v>
       </c>
       <c r="X20">
-        <v>645.932635147256</v>
+        <v>1646.413439253672</v>
       </c>
       <c r="Y20">
-        <v>1.248180737705653</v>
+        <v>0.9934269321873943</v>
       </c>
       <c r="Z20">
-        <v>1410.001659557441</v>
+        <v>1410.26521208802</v>
       </c>
       <c r="AA20">
-        <v>908.8896194195452</v>
+        <v>2180.473317499082</v>
       </c>
       <c r="AB20">
-        <v>1.023835340487125</v>
+        <v>0.8314880317421872</v>
       </c>
       <c r="AC20">
-        <v>1370.618511303125</v>
+        <v>1370.713680696468</v>
       </c>
       <c r="AD20">
-        <v>119.9079030005159</v>
+        <v>327.5447717095616</v>
       </c>
       <c r="AE20">
-        <v>0.3800751321017891</v>
+        <v>0.3393058662925294</v>
       </c>
     </row>
     <row r="21" spans="1:31">
@@ -2396,88 +2366,88 @@
         <v>49</v>
       </c>
       <c r="C21">
-        <v>103.1904595631331</v>
+        <v>102.9777594827942</v>
       </c>
       <c r="D21">
-        <v>1285.554182574357</v>
+        <v>1286.056143914295</v>
       </c>
       <c r="E21">
-        <v>2258.212989566675</v>
+        <v>6193.434332155342</v>
       </c>
       <c r="F21">
-        <v>1285.554232576857</v>
+        <v>1286.056193916795</v>
       </c>
       <c r="G21">
-        <v>4975.600082279964</v>
+        <v>11516.32511221137</v>
       </c>
       <c r="H21">
-        <v>0.8450390720076749</v>
+        <v>0.7365539142136411</v>
       </c>
       <c r="I21">
-        <v>3.77361761925854</v>
+        <v>8.063929049956968</v>
       </c>
       <c r="J21">
-        <v>0.574497792300012</v>
+        <v>0.4865237108152374</v>
       </c>
       <c r="K21">
-        <v>1.69007814401535</v>
+        <v>1.473107828427282</v>
       </c>
       <c r="L21" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M21">
-        <v>1388.74464213749</v>
+        <v>1389.03400340209</v>
       </c>
       <c r="N21">
-        <v>4071.890064826601</v>
+        <v>10280.97239748438</v>
       </c>
       <c r="O21">
-        <v>1388.744692139991</v>
+        <v>1389.03395339959</v>
       </c>
       <c r="P21">
-        <v>7700.113141464022</v>
+        <v>17126.28689687452</v>
       </c>
       <c r="Q21">
-        <v>0.7347875675801828</v>
+        <v>0.6722101212806841</v>
       </c>
       <c r="S21">
-        <v>4.403274357649957</v>
+        <v>9.370544878994155</v>
       </c>
       <c r="T21">
-        <v>0.5372326738508525</v>
+        <v>0.4373620193254469</v>
       </c>
       <c r="U21">
-        <v>1.469575135160366</v>
+        <v>1.344420242561368</v>
       </c>
       <c r="V21" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W21">
-        <v>1265.4157685937</v>
+        <v>1265.842995337195</v>
       </c>
       <c r="X21">
-        <v>585.6005303355907</v>
+        <v>1330.732876355486</v>
       </c>
       <c r="Y21">
-        <v>1.164376554890733</v>
+        <v>0.9234993920455057</v>
       </c>
       <c r="Z21">
-        <v>1410.073376335864</v>
+        <v>1410.32543609367</v>
       </c>
       <c r="AA21">
-        <v>779.4617018826613</v>
+        <v>1776.865379774378</v>
       </c>
       <c r="AB21">
-        <v>0.9511840237399525</v>
+        <v>0.7940698511159414</v>
       </c>
       <c r="AC21">
-        <v>1370.672271732659</v>
+        <v>1370.735536357876</v>
       </c>
       <c r="AD21">
-        <v>117.2660636989927</v>
+        <v>279.2075659735946</v>
       </c>
       <c r="AE21">
-        <v>0.3669392440496521</v>
+        <v>0.3358381772225094</v>
       </c>
     </row>
     <row r="22" spans="1:31">
@@ -2488,88 +2458,88 @@
         <v>50</v>
       </c>
       <c r="C22">
-        <v>103.1252545199534</v>
+        <v>102.9517299758602</v>
       </c>
       <c r="D22">
-        <v>1285.703640780499</v>
+        <v>1286.136938619289</v>
       </c>
       <c r="E22">
-        <v>2057.431550309846</v>
+        <v>4882.921838000918</v>
       </c>
       <c r="F22">
-        <v>1285.703690782999</v>
+        <v>1286.136988621789</v>
       </c>
       <c r="G22">
-        <v>4377.479702877658</v>
+        <v>8767.235086272933</v>
       </c>
       <c r="H22">
-        <v>0.8207457698549424</v>
+        <v>0.7117310844527485</v>
       </c>
       <c r="I22">
-        <v>3.732879547035927</v>
+        <v>7.962427752501213</v>
       </c>
       <c r="J22">
-        <v>0.5554259365161527</v>
+        <v>0.4846303562235565</v>
       </c>
       <c r="K22">
-        <v>1.641491539709885</v>
+        <v>1.423462168905497</v>
       </c>
       <c r="L22" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M22">
-        <v>1388.828895300452</v>
+        <v>1389.088768600149</v>
       </c>
       <c r="N22">
-        <v>3708.300995887869</v>
+        <v>7895.790584796339</v>
       </c>
       <c r="O22">
-        <v>1388.828945302952</v>
+        <v>1389.088718597649</v>
       </c>
       <c r="P22">
-        <v>6739.279705437903</v>
+        <v>12720.55030754296</v>
       </c>
       <c r="Q22">
-        <v>0.7110504784543589</v>
+        <v>0.6573666631512465</v>
       </c>
       <c r="S22">
-        <v>3.489812033682869</v>
+        <v>7.165476931567271</v>
       </c>
       <c r="T22">
-        <v>0.5193172598163406</v>
+        <v>0.4075745519007695</v>
       </c>
       <c r="U22">
-        <v>1.422100956908718</v>
+        <v>1.314733326302493</v>
       </c>
       <c r="V22" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W22">
-        <v>1265.547179499557</v>
+        <v>1265.913182388908</v>
       </c>
       <c r="X22">
-        <v>519.0681363087882</v>
+        <v>1017.925863136379</v>
       </c>
       <c r="Y22">
-        <v>1.17529156762116</v>
+        <v>0.9052157404514666</v>
       </c>
       <c r="Z22">
-        <v>1410.087688894596</v>
+        <v>1410.376250167117</v>
       </c>
       <c r="AA22">
-        <v>664.1469029764719</v>
+        <v>1322.764691421511</v>
       </c>
       <c r="AB22">
-        <v>0.8705165787787821</v>
+        <v>0.7787587478973595</v>
       </c>
       <c r="AC22">
-        <v>1370.674506724649</v>
+        <v>1370.727506080769</v>
       </c>
       <c r="AD22">
-        <v>89.40409401854464</v>
+        <v>195.8339840424975</v>
       </c>
       <c r="AE22">
-        <v>0.3549350518284763</v>
+        <v>0.3284658743364031</v>
       </c>
     </row>
     <row r="23" spans="1:31">
@@ -2580,88 +2550,88 @@
         <v>51</v>
       </c>
       <c r="C23">
-        <v>103.0191423929543</v>
+        <v>102.9201272843125</v>
       </c>
       <c r="D23">
-        <v>1285.956349579502</v>
+        <v>1286.225653618336</v>
       </c>
       <c r="E23">
-        <v>7070.532681252636</v>
+        <v>4277.161705120281</v>
       </c>
       <c r="F23">
-        <v>1285.956399582002</v>
+        <v>1286.225703620836</v>
       </c>
       <c r="G23">
-        <v>13657.39850773385</v>
+        <v>7359.674651348743</v>
       </c>
       <c r="H23">
-        <v>0.765399293674688</v>
+        <v>0.6899214952843491</v>
       </c>
       <c r="I23">
-        <v>9.593159512802318</v>
+        <v>6.926748209277338</v>
       </c>
       <c r="J23">
-        <v>0.4883629215121236</v>
+        <v>0.4544737223663027</v>
       </c>
       <c r="K23">
-        <v>1.530798587349376</v>
+        <v>1.379842990568698</v>
       </c>
       <c r="L23" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M23">
-        <v>1388.975491972456</v>
+        <v>1389.145880907648</v>
       </c>
       <c r="N23">
-        <v>12148.82995333333</v>
+        <v>6778.168399766881</v>
       </c>
       <c r="O23">
-        <v>1388.975541974957</v>
+        <v>1389.145830905148</v>
       </c>
       <c r="P23">
-        <v>20609.16538832924</v>
+        <v>10694.9553791159</v>
       </c>
       <c r="Q23">
-        <v>0.6796022340646839</v>
+        <v>0.650718190921989</v>
       </c>
       <c r="S23">
-        <v>10.40173571365554</v>
+        <v>6.322317125841809</v>
       </c>
       <c r="T23">
-        <v>0.4585767800724904</v>
+        <v>0.378693651926219</v>
       </c>
       <c r="U23">
-        <v>1.359204468129368</v>
+        <v>1.301436381843978</v>
       </c>
       <c r="V23" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W23">
-        <v>1265.749091708977</v>
+        <v>1266.012026560361</v>
       </c>
       <c r="X23">
-        <v>1549.899201572086</v>
+        <v>831.0275815813417</v>
       </c>
       <c r="Y23">
-        <v>0.9396337780991795</v>
+        <v>0.8186118424480687</v>
       </c>
       <c r="Z23">
-        <v>1410.26572892124</v>
+        <v>1410.420038643695</v>
       </c>
       <c r="AA23">
-        <v>2134.143938151425</v>
+        <v>1113.756223528605</v>
       </c>
       <c r="AB23">
-        <v>0.8315296639829045</v>
+        <v>0.7474737112567265</v>
       </c>
       <c r="AC23">
-        <v>1370.712667417209</v>
+        <v>1370.77142810503</v>
       </c>
       <c r="AD23">
-        <v>315.3096097091661</v>
+        <v>166.4838028356527</v>
       </c>
       <c r="AE23">
-        <v>0.3380544825803046</v>
+        <v>0.3251508773415833</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -2672,88 +2642,88 @@
         <v>52</v>
       </c>
       <c r="C24">
-        <v>102.9774691452631</v>
+        <v>102.8854867209184</v>
       </c>
       <c r="D24">
-        <v>1286.056110113841</v>
+        <v>1286.307951540531</v>
       </c>
       <c r="E24">
-        <v>6189.163706113585</v>
+        <v>3730.036984547919</v>
       </c>
       <c r="F24">
-        <v>1286.056160116342</v>
+        <v>1286.308001543031</v>
       </c>
       <c r="G24">
-        <v>11486.22573292251</v>
+        <v>6286.535850655989</v>
       </c>
       <c r="H24">
-        <v>0.736783281071772</v>
+        <v>0.6896631206915288</v>
       </c>
       <c r="I24">
-        <v>7.433583671362237</v>
+        <v>5.957988302554774</v>
       </c>
       <c r="J24">
-        <v>0.4807504808455313</v>
+        <v>0.3999690694606421</v>
       </c>
       <c r="K24">
-        <v>1.473566562143544</v>
+        <v>1.379326241383058</v>
       </c>
       <c r="L24" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M24">
-        <v>1389.033779269105</v>
+        <v>1389.193538266449</v>
       </c>
       <c r="N24">
-        <v>10276.23910014301</v>
+        <v>5897.922677114351</v>
       </c>
       <c r="O24">
-        <v>1389.033629261605</v>
+        <v>1389.193488263949</v>
       </c>
       <c r="P24">
-        <v>16883.99350221537</v>
+        <v>9078.622209932817</v>
       </c>
       <c r="Q24">
-        <v>0.6707241467118706</v>
+        <v>0.6347943001506124</v>
       </c>
       <c r="S24">
-        <v>9.378973815252712</v>
+        <v>5.941475301992425</v>
       </c>
       <c r="T24">
-        <v>0.4174569310394609</v>
+        <v>0.3787672072448742</v>
       </c>
       <c r="U24">
-        <v>1.341448293423741</v>
+        <v>1.269588600301225</v>
       </c>
       <c r="V24" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W24">
-        <v>1265.843062437174</v>
+        <v>1266.04970179604</v>
       </c>
       <c r="X24">
-        <v>1309.119171229104</v>
+        <v>708.7266170706818</v>
       </c>
       <c r="Y24">
-        <v>0.9155085701439718</v>
+        <v>0.7479371156317673</v>
       </c>
       <c r="Z24">
-        <v>1410.325322414572</v>
+        <v>1410.465766809849</v>
       </c>
       <c r="AA24">
-        <v>1765.372849559903</v>
+        <v>944.0256766249922</v>
       </c>
       <c r="AB24">
-        <v>0.793961996976859</v>
+        <v>0.678920395512001</v>
       </c>
       <c r="AC24">
-        <v>1370.735471159083</v>
+        <v>1370.785392494354</v>
       </c>
       <c r="AD24">
-        <v>282.7206707450472</v>
+        <v>139.7862394548568</v>
       </c>
       <c r="AE24">
-        <v>0.335836912617819</v>
+        <v>0.3171735685656548</v>
       </c>
     </row>
     <row r="25" spans="1:31">
@@ -2764,88 +2734,88 @@
         <v>53</v>
       </c>
       <c r="C25">
-        <v>102.9512869607163</v>
+        <v>102.8590920425645</v>
       </c>
       <c r="D25">
-        <v>1286.136960281237</v>
+        <v>1286.380006293332</v>
       </c>
       <c r="E25">
-        <v>4876.509375600772</v>
+        <v>3195.521434037692</v>
       </c>
       <c r="F25">
-        <v>1286.136910278737</v>
+        <v>1286.380056295832</v>
       </c>
       <c r="G25">
-        <v>8720.905860460605</v>
+        <v>5186.596009202736</v>
       </c>
       <c r="H25">
-        <v>0.7121752078034486</v>
+        <v>0.6687518113403557</v>
       </c>
       <c r="I25">
-        <v>7.51764806674078</v>
+        <v>6.138489029197251</v>
       </c>
       <c r="J25">
-        <v>0.4734283748153258</v>
+        <v>0.3813098973172788</v>
       </c>
       <c r="K25">
-        <v>1.424350415606897</v>
+        <v>1.337503622680711</v>
       </c>
       <c r="L25" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M25">
-        <v>1389.088347246953</v>
+        <v>1389.239198340897</v>
       </c>
       <c r="N25">
-        <v>7891.72728537596</v>
+        <v>4929.191802149563</v>
       </c>
       <c r="O25">
-        <v>1389.088197239453</v>
+        <v>1389.239148338397</v>
       </c>
       <c r="P25">
-        <v>12480.10835877858</v>
+        <v>7402.292866098572</v>
       </c>
       <c r="Q25">
-        <v>0.6553563473701567</v>
+        <v>0.6218421617889781</v>
       </c>
       <c r="S25">
-        <v>7.156050149966658</v>
+        <v>5.396228049801347</v>
       </c>
       <c r="T25">
-        <v>0.380426360405032</v>
+        <v>0.3675695307706013</v>
       </c>
       <c r="U25">
-        <v>1.310712694740313</v>
+        <v>1.243684323577956</v>
       </c>
       <c r="V25" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W25">
-        <v>1265.913115814039</v>
+        <v>1266.148667124799</v>
       </c>
       <c r="X25">
-        <v>988.559390384248</v>
+        <v>584.600951578361</v>
       </c>
       <c r="Y25">
-        <v>0.8968688852170305</v>
+        <v>0.7720993401726601</v>
       </c>
       <c r="Z25">
-        <v>1410.376092646718</v>
+        <v>1410.505925101817</v>
       </c>
       <c r="AA25">
-        <v>1316.350896067387</v>
+        <v>757.8718575680169</v>
       </c>
       <c r="AB25">
-        <v>0.7787150814373053</v>
+        <v>0.6650456142472337</v>
       </c>
       <c r="AC25">
-        <v>1370.727491433549</v>
+        <v>1370.783044405585</v>
       </c>
       <c r="AD25">
-        <v>198.3175371533952</v>
+        <v>104.0335331210563</v>
       </c>
       <c r="AE25">
-        <v>0.3284677270054002</v>
+        <v>0.3106807713082378</v>
       </c>
     </row>
     <row r="26" spans="1:31">
@@ -2856,88 +2826,88 @@
         <v>54</v>
       </c>
       <c r="C26">
-        <v>102.9202305620536</v>
+        <v>102.8338158453857</v>
       </c>
       <c r="D26">
-        <v>1286.224885421594</v>
+        <v>1286.448209381442</v>
       </c>
       <c r="E26">
-        <v>4265.553184239407</v>
+        <v>2444.588298549893</v>
       </c>
       <c r="F26">
-        <v>1286.224435399093</v>
+        <v>1286.448259383943</v>
       </c>
       <c r="G26">
-        <v>7112.514840092621</v>
+        <v>3858.038117403481</v>
       </c>
       <c r="H26">
-        <v>0.6882012855729107</v>
+        <v>0.6592552609221147</v>
       </c>
       <c r="I26">
-        <v>6.636826490080628</v>
+        <v>4.487930627675135</v>
       </c>
       <c r="J26">
-        <v>0.4001013293753136</v>
+        <v>0.3435898277223514</v>
       </c>
       <c r="K26">
-        <v>1.376402571145821</v>
+        <v>1.318510521844229</v>
       </c>
       <c r="L26" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="M26">
-        <v>1389.145015978648</v>
+        <v>1389.282125231828</v>
       </c>
       <c r="N26">
-        <v>6771.754857318544</v>
+        <v>3853.318076049098</v>
       </c>
       <c r="O26">
-        <v>1389.144665961147</v>
+        <v>1389.282075229328</v>
       </c>
       <c r="P26">
-        <v>10350.15993319062</v>
+        <v>5632.412666133469</v>
       </c>
       <c r="Q26">
-        <v>0.6475054788019109</v>
+        <v>0.6106053109672093</v>
       </c>
       <c r="S26">
-        <v>6.300865090329574</v>
+        <v>4.722163652505605</v>
       </c>
       <c r="T26">
-        <v>0.3301160725727898</v>
+        <v>0.3434617724180289</v>
       </c>
       <c r="U26">
-        <v>1.295010957603822</v>
+        <v>1.221210621934419</v>
       </c>
       <c r="V26" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="W26">
-        <v>1266.012338461197</v>
+        <v>1266.173729303071</v>
       </c>
       <c r="X26">
-        <v>820.4423045677801</v>
+        <v>409.4358723092514</v>
       </c>
       <c r="Y26">
-        <v>0.8171997127388795</v>
+        <v>0.7778723355050303</v>
       </c>
       <c r="Z26">
-        <v>1410.419960932707</v>
+        <v>1410.546932073475</v>
       </c>
       <c r="AA26">
-        <v>1116.598001068766</v>
+        <v>576.7937833608</v>
       </c>
       <c r="AB26">
-        <v>0.7473907391169377</v>
+        <v>0.6678558384561352</v>
       </c>
       <c r="AC26">
-        <v>1370.771143457551</v>
+        <v>1370.79478629867</v>
       </c>
       <c r="AD26">
-        <v>167.6844558923569</v>
+        <v>76.34155790860562</v>
       </c>
       <c r="AE26">
-        <v>0.3251526865694079</v>
+        <v>0.3050286413555269</v>
       </c>
     </row>
     <row r="27" spans="1:31">
@@ -2948,88 +2918,1562 @@
         <v>55</v>
       </c>
       <c r="C27">
-        <v>104.3844424662975</v>
+        <v>102.8110892174454</v>
       </c>
       <c r="D27">
-        <v>1282.849918288139</v>
+        <v>1286.490981178844</v>
       </c>
       <c r="E27">
-        <v>3948.219488668278</v>
+        <v>2228.792539688438</v>
       </c>
       <c r="F27">
-        <v>1282.849768280639</v>
+        <v>1286.491031181344</v>
       </c>
       <c r="G27">
-        <v>11938.37320476673</v>
+        <v>3464.02842708066</v>
       </c>
       <c r="H27">
-        <v>1.10770010995593</v>
+        <v>0.6522092191014404</v>
       </c>
       <c r="I27">
-        <v>5.468284362713543</v>
+        <v>4.222827661824773</v>
       </c>
       <c r="J27">
-        <v>0.6953317184857992</v>
+        <v>0.3309559221069815</v>
       </c>
       <c r="K27">
-        <v>2.21540021991186</v>
+        <v>1.304418438202881</v>
       </c>
       <c r="L27" t="s">
+        <v>73</v>
+      </c>
+      <c r="M27">
+        <v>1389.30217040129</v>
+      </c>
+      <c r="N27">
+        <v>3451.733759487993</v>
+      </c>
+      <c r="O27">
+        <v>1389.30212039879</v>
+      </c>
+      <c r="P27">
+        <v>4984.665941607343</v>
+      </c>
+      <c r="Q27">
+        <v>0.6104890436481539</v>
+      </c>
+      <c r="S27">
+        <v>5.196066635318773</v>
+      </c>
+      <c r="T27">
+        <v>0.3103324780151462</v>
+      </c>
+      <c r="U27">
+        <v>1.220978087296308</v>
+      </c>
+      <c r="V27" t="s">
+        <v>73</v>
+      </c>
+      <c r="W27">
+        <v>1266.233080319655</v>
+      </c>
+      <c r="X27">
+        <v>361.2219396908037</v>
+      </c>
+      <c r="Y27">
+        <v>0.7685277702898632</v>
+      </c>
+      <c r="Z27">
+        <v>1410.568766673513</v>
+      </c>
+      <c r="AA27">
+        <v>507.7837340013061</v>
+      </c>
+      <c r="AB27">
+        <v>0.6155910820992763</v>
+      </c>
+      <c r="AC27">
+        <v>1369.72634991542</v>
+      </c>
+      <c r="AD27">
+        <v>18.22104370593397</v>
+      </c>
+      <c r="AE27">
+        <v>0.3049853878440121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
+      <c r="A28" s="1">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
         <v>56</v>
       </c>
-      <c r="M27">
-        <v>1387.234260749436</v>
-      </c>
-      <c r="N27">
-        <v>7766.002243055656</v>
-      </c>
-      <c r="O27">
-        <v>1387.234210746936</v>
-      </c>
-      <c r="P27">
-        <v>21307.31431584729</v>
-      </c>
-      <c r="Q27">
-        <v>0.9790751374941751</v>
-      </c>
-      <c r="S27">
-        <v>10.89885110399582</v>
-      </c>
-      <c r="T27">
-        <v>0.7469423768322202</v>
-      </c>
-      <c r="U27">
-        <v>1.95815027498835</v>
-      </c>
-      <c r="V27" t="s">
-        <v>56</v>
-      </c>
-      <c r="W27">
-        <v>1262.806659888847</v>
-      </c>
-      <c r="X27">
-        <v>1742.242120977632</v>
-      </c>
-      <c r="Y27">
-        <v>2.976448947927353</v>
-      </c>
-      <c r="Z27">
-        <v>1408.519811657963</v>
-      </c>
-      <c r="AA27">
-        <v>2465.360576075262</v>
-      </c>
-      <c r="AB27">
-        <v>2.476882169786846</v>
-      </c>
-      <c r="AC27">
-        <v>1369.65176005707</v>
-      </c>
-      <c r="AD27">
-        <v>334.2775638593454</v>
-      </c>
-      <c r="AE27">
-        <v>0.4885990715615605</v>
+      <c r="C28">
+        <v>102.8075039445264</v>
+      </c>
+      <c r="D28">
+        <v>1286.514200776782</v>
+      </c>
+      <c r="E28">
+        <v>2008.914152700353</v>
+      </c>
+      <c r="F28">
+        <v>1286.514250779283</v>
+      </c>
+      <c r="G28">
+        <v>3122.915378257817</v>
+      </c>
+      <c r="H28">
+        <v>0.6526553224275554</v>
+      </c>
+      <c r="I28">
+        <v>4.204856798142449</v>
+      </c>
+      <c r="J28">
+        <v>0.3296167102137692</v>
+      </c>
+      <c r="K28">
+        <v>1.305310644855111</v>
+      </c>
+      <c r="L28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M28">
+        <v>1389.321804726309</v>
+      </c>
+      <c r="N28">
+        <v>3155.938035646115</v>
+      </c>
+      <c r="O28">
+        <v>1389.321754723809</v>
+      </c>
+      <c r="P28">
+        <v>4512.979450633281</v>
+      </c>
+      <c r="Q28">
+        <v>0.6017178706961606</v>
+      </c>
+      <c r="S28">
+        <v>4.429979598086735</v>
+      </c>
+      <c r="T28">
+        <v>0.3233058552558019</v>
+      </c>
+      <c r="U28">
+        <v>1.203435741392321</v>
+      </c>
+      <c r="V28" t="s">
+        <v>73</v>
+      </c>
+      <c r="W28">
+        <v>1266.227156007076</v>
+      </c>
+      <c r="X28">
+        <v>333.6920204770568</v>
+      </c>
+      <c r="Y28">
+        <v>0.748528541826977</v>
+      </c>
+      <c r="Z28">
+        <v>1410.567459936427</v>
+      </c>
+      <c r="AA28">
+        <v>459.1396439693752</v>
+      </c>
+      <c r="AB28">
+        <v>0.6469907778817845</v>
+      </c>
+      <c r="AC28">
+        <v>1370.782119851041</v>
+      </c>
+      <c r="AD28">
+        <v>66.1382690430605</v>
+      </c>
+      <c r="AE28">
+        <v>0.3005433826960575</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
+      <c r="A29" s="1">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29">
+        <v>102.8040319114118</v>
+      </c>
+      <c r="D29">
+        <v>1286.536065119207</v>
+      </c>
+      <c r="E29">
+        <v>1867.856382204665</v>
+      </c>
+      <c r="F29">
+        <v>1286.536115121707</v>
+      </c>
+      <c r="G29">
+        <v>2833.767428115432</v>
+      </c>
+      <c r="H29">
+        <v>0.6438414418207397</v>
+      </c>
+      <c r="I29">
+        <v>4.781712560499805</v>
+      </c>
+      <c r="J29">
+        <v>0.2996295387127584</v>
+      </c>
+      <c r="K29">
+        <v>1.287682883641479</v>
+      </c>
+      <c r="L29" t="s">
+        <v>73</v>
+      </c>
+      <c r="M29">
+        <v>1389.340197035619</v>
+      </c>
+      <c r="N29">
+        <v>2911.813173124914</v>
+      </c>
+      <c r="O29">
+        <v>1389.340147033119</v>
+      </c>
+      <c r="P29">
+        <v>4093.336226548224</v>
+      </c>
+      <c r="Q29">
+        <v>0.5958447846143755</v>
+      </c>
+      <c r="S29">
+        <v>3.650170321357557</v>
+      </c>
+      <c r="T29">
+        <v>0.3029849297444478</v>
+      </c>
+      <c r="U29">
+        <v>1.191689569228751</v>
+      </c>
+      <c r="V29" t="s">
+        <v>73</v>
+      </c>
+      <c r="W29">
+        <v>1266.272881965968</v>
+      </c>
+      <c r="X29">
+        <v>314.2119957699144</v>
+      </c>
+      <c r="Y29">
+        <v>0.6964657444726008</v>
+      </c>
+      <c r="Z29">
+        <v>1410.586537276874</v>
+      </c>
+      <c r="AA29">
+        <v>415.9351103070103</v>
+      </c>
+      <c r="AB29">
+        <v>0.6313792902480254</v>
+      </c>
+      <c r="AC29">
+        <v>1371.162969525947</v>
+      </c>
+      <c r="AD29">
+        <v>53.60085927999295</v>
+      </c>
+      <c r="AE29">
+        <v>0.2976151037944949</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
+      <c r="A30" s="1">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30">
+        <v>102.7771984309838</v>
+      </c>
+      <c r="D30">
+        <v>1286.565650661038</v>
+      </c>
+      <c r="E30">
+        <v>1583.914898517135</v>
+      </c>
+      <c r="F30">
+        <v>1286.565700663538</v>
+      </c>
+      <c r="G30">
+        <v>2353.192301141593</v>
+      </c>
+      <c r="H30">
+        <v>0.6309318462499222</v>
+      </c>
+      <c r="I30">
+        <v>3.40890921546771</v>
+      </c>
+      <c r="J30">
+        <v>0.297688179092971</v>
+      </c>
+      <c r="K30">
+        <v>1.261863692499844</v>
+      </c>
+      <c r="L30" t="s">
+        <v>73</v>
+      </c>
+      <c r="M30">
+        <v>1389.342949097022</v>
+      </c>
+      <c r="N30">
+        <v>2494.72909091248</v>
+      </c>
+      <c r="O30">
+        <v>1389.342899094522</v>
+      </c>
+      <c r="P30">
+        <v>3472.020318240124</v>
+      </c>
+      <c r="Q30">
+        <v>0.5870947450132744</v>
+      </c>
+      <c r="S30">
+        <v>4.062168166848709</v>
+      </c>
+      <c r="T30">
+        <v>0.3163200629147129</v>
+      </c>
+      <c r="U30">
+        <v>1.174189490026549</v>
+      </c>
+      <c r="V30" t="s">
+        <v>73</v>
+      </c>
+      <c r="W30">
+        <v>1266.288328431901</v>
+      </c>
+      <c r="X30">
+        <v>260.4103553883812</v>
+      </c>
+      <c r="Y30">
+        <v>0.683449397976062</v>
+      </c>
+      <c r="Z30">
+        <v>1410.61720066604</v>
+      </c>
+      <c r="AA30">
+        <v>356.7239957002217</v>
+      </c>
+      <c r="AB30">
+        <v>0.6222077956460655</v>
+      </c>
+      <c r="AC30">
+        <v>1371.181254280111</v>
+      </c>
+      <c r="AD30">
+        <v>43.97108933341576</v>
+      </c>
+      <c r="AE30">
+        <v>0.2932137035071767</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31">
+        <v>102.7813879471662</v>
+      </c>
+      <c r="D31">
+        <v>1286.584352078927</v>
+      </c>
+      <c r="E31">
+        <v>1310.046828608404</v>
+      </c>
+      <c r="F31">
+        <v>1286.584402081427</v>
+      </c>
+      <c r="G31">
+        <v>1945.263849629274</v>
+      </c>
+      <c r="H31">
+        <v>0.6381558033296094</v>
+      </c>
+      <c r="I31">
+        <v>2.870312190702393</v>
+      </c>
+      <c r="J31">
+        <v>0.2639654763261385</v>
+      </c>
+      <c r="K31">
+        <v>1.276311606659219</v>
+      </c>
+      <c r="L31" t="s">
+        <v>73</v>
+      </c>
+      <c r="M31">
+        <v>1389.365840031094</v>
+      </c>
+      <c r="N31">
+        <v>2062.334556296285</v>
+      </c>
+      <c r="O31">
+        <v>1389.365790028593</v>
+      </c>
+      <c r="P31">
+        <v>2832.395327341664</v>
+      </c>
+      <c r="Q31">
+        <v>0.5910012832769235</v>
+      </c>
+      <c r="S31">
+        <v>3.059275416795949</v>
+      </c>
+      <c r="T31">
+        <v>0.2602586776726156</v>
+      </c>
+      <c r="U31">
+        <v>1.182002566553847</v>
+      </c>
+      <c r="V31" t="s">
+        <v>73</v>
+      </c>
+      <c r="W31">
+        <v>1266.315192726646</v>
+      </c>
+      <c r="X31">
+        <v>191.0196532078688</v>
+      </c>
+      <c r="Y31">
+        <v>0.7148681115661863</v>
+      </c>
+      <c r="Z31">
+        <v>1410.613950953094</v>
+      </c>
+      <c r="AA31">
+        <v>268.0763099178611</v>
+      </c>
+      <c r="AB31">
+        <v>0.6184440183899719</v>
+      </c>
+      <c r="AC31">
+        <v>1371.172615708342</v>
+      </c>
+      <c r="AD31">
+        <v>37.01143129613941</v>
+      </c>
+      <c r="AE31">
+        <v>0.2952012310146522</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
+      <c r="A32" s="1">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>102.771354485265</v>
+      </c>
+      <c r="D32">
+        <v>1286.598053797721</v>
+      </c>
+      <c r="E32">
+        <v>1088.256617469049</v>
+      </c>
+      <c r="F32">
+        <v>1286.598103800221</v>
+      </c>
+      <c r="G32">
+        <v>1595.735134705747</v>
+      </c>
+      <c r="H32">
+        <v>0.6327017920386042</v>
+      </c>
+      <c r="I32">
+        <v>2.770988230852673</v>
+      </c>
+      <c r="J32">
+        <v>0.252602537008485</v>
+      </c>
+      <c r="K32">
+        <v>1.265403584077208</v>
+      </c>
+      <c r="L32" t="s">
+        <v>73</v>
+      </c>
+      <c r="M32">
+        <v>1389.369508287986</v>
+      </c>
+      <c r="N32">
+        <v>1731.163450550091</v>
+      </c>
+      <c r="O32">
+        <v>1389.369458285486</v>
+      </c>
+      <c r="P32">
+        <v>2381.736286683175</v>
+      </c>
+      <c r="Q32">
+        <v>0.596015743775793</v>
+      </c>
+      <c r="S32">
+        <v>2.791249296877861</v>
+      </c>
+      <c r="T32">
+        <v>0.2411697897755906</v>
+      </c>
+      <c r="U32">
+        <v>1.192031487551586</v>
+      </c>
+      <c r="V32" t="s">
+        <v>73</v>
+      </c>
+      <c r="W32">
+        <v>1266.305772267469</v>
+      </c>
+      <c r="X32">
+        <v>159.1139128954202</v>
+      </c>
+      <c r="Y32">
+        <v>0.6917744731424587</v>
+      </c>
+      <c r="Z32">
+        <v>1410.597241348</v>
+      </c>
+      <c r="AA32">
+        <v>229.2143768369037</v>
+      </c>
+      <c r="AB32">
+        <v>0.6093492876262875</v>
+      </c>
+      <c r="AC32">
+        <v>1371.193576253521</v>
+      </c>
+      <c r="AD32">
+        <v>34.95354610374938</v>
+      </c>
+      <c r="AE32">
+        <v>0.2976941071922947</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31">
+      <c r="A33" s="1">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33">
+        <v>102.7690053065423</v>
+      </c>
+      <c r="D33">
+        <v>1286.609901163167</v>
+      </c>
+      <c r="E33">
+        <v>1029.254549679472</v>
+      </c>
+      <c r="F33">
+        <v>1286.609951165668</v>
+      </c>
+      <c r="G33">
+        <v>1500.313799500764</v>
+      </c>
+      <c r="H33">
+        <v>0.6237613931797109</v>
+      </c>
+      <c r="I33">
+        <v>2.522790411698803</v>
+      </c>
+      <c r="J33">
+        <v>0.2762470051906702</v>
+      </c>
+      <c r="K33">
+        <v>1.247522786359422</v>
+      </c>
+      <c r="L33" t="s">
+        <v>73</v>
+      </c>
+      <c r="M33">
+        <v>1389.37890646971</v>
+      </c>
+      <c r="N33">
+        <v>1590.057836208822</v>
+      </c>
+      <c r="O33">
+        <v>1389.37895647221</v>
+      </c>
+      <c r="P33">
+        <v>2173.014262660829</v>
+      </c>
+      <c r="Q33">
+        <v>0.5910026568398647</v>
+      </c>
+      <c r="S33">
+        <v>2.518308663699042</v>
+      </c>
+      <c r="T33">
+        <v>0.2461475351533907</v>
+      </c>
+      <c r="U33">
+        <v>1.182005313679729</v>
+      </c>
+      <c r="V33" t="s">
+        <v>73</v>
+      </c>
+      <c r="W33">
+        <v>1266.332772710224</v>
+      </c>
+      <c r="X33">
+        <v>157.9681052174095</v>
+      </c>
+      <c r="Y33">
+        <v>0.6127680337824004</v>
+      </c>
+      <c r="Z33">
+        <v>1410.62333957808</v>
+      </c>
+      <c r="AA33">
+        <v>192.3681783160284</v>
+      </c>
+      <c r="AB33">
+        <v>0.6388171059759475</v>
+      </c>
+      <c r="AC33">
+        <v>1370.815893004649</v>
+      </c>
+      <c r="AD33">
+        <v>27.99055711271873</v>
+      </c>
+      <c r="AE33">
+        <v>0.295235138826219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31">
+      <c r="A34" s="1">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34">
+        <v>102.7603007143803</v>
+      </c>
+      <c r="D34">
+        <v>1286.618257532714</v>
+      </c>
+      <c r="E34">
+        <v>869.1145629129204</v>
+      </c>
+      <c r="F34">
+        <v>1286.618307535214</v>
+      </c>
+      <c r="G34">
+        <v>1250.242995652173</v>
+      </c>
+      <c r="H34">
+        <v>0.6332230987888853</v>
+      </c>
+      <c r="I34">
+        <v>2.456907951536023</v>
+      </c>
+      <c r="J34">
+        <v>0.1951168972700147</v>
+      </c>
+      <c r="K34">
+        <v>1.266446197577771</v>
+      </c>
+      <c r="L34" t="s">
+        <v>73</v>
+      </c>
+      <c r="M34">
+        <v>1389.378658252094</v>
+      </c>
+      <c r="N34">
+        <v>1387.397975698949</v>
+      </c>
+      <c r="O34">
+        <v>1389.378608249594</v>
+      </c>
+      <c r="P34">
+        <v>1880.244517855218</v>
+      </c>
+      <c r="Q34">
+        <v>0.5846950630966414</v>
+      </c>
+      <c r="S34">
+        <v>2.283209302925246</v>
+      </c>
+      <c r="T34">
+        <v>0.2528779191228955</v>
+      </c>
+      <c r="U34">
+        <v>1.169390126193283</v>
+      </c>
+      <c r="V34" t="s">
+        <v>73</v>
+      </c>
+      <c r="W34">
+        <v>1266.318666400476</v>
+      </c>
+      <c r="X34">
+        <v>122.4809978310145</v>
+      </c>
+      <c r="Y34">
+        <v>0.6949021055582221</v>
+      </c>
+      <c r="Z34">
+        <v>1410.618828158267</v>
+      </c>
+      <c r="AA34">
+        <v>170.7078030237925</v>
+      </c>
+      <c r="AB34">
+        <v>0.6192840050628398</v>
+      </c>
+      <c r="AC34">
+        <v>1371.19299997035</v>
+      </c>
+      <c r="AD34">
+        <v>26.23408133876216</v>
+      </c>
+      <c r="AE34">
+        <v>0.2920530324144043</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35">
+        <v>102.7539090953737</v>
+      </c>
+      <c r="D35">
+        <v>1286.643881035681</v>
+      </c>
+      <c r="E35">
+        <v>644.8889445499187</v>
+      </c>
+      <c r="F35">
+        <v>1286.643931038181</v>
+      </c>
+      <c r="G35">
+        <v>903.9231600748495</v>
+      </c>
+      <c r="H35">
+        <v>0.6164964765488484</v>
+      </c>
+      <c r="I35">
+        <v>2.079446683855339</v>
+      </c>
+      <c r="J35">
+        <v>0.1974303432814151</v>
+      </c>
+      <c r="K35">
+        <v>1.232992953097697</v>
+      </c>
+      <c r="L35" t="s">
+        <v>73</v>
+      </c>
+      <c r="M35">
+        <v>1389.397890136055</v>
+      </c>
+      <c r="N35">
+        <v>1012.261940567408</v>
+      </c>
+      <c r="O35">
+        <v>1389.397840133555</v>
+      </c>
+      <c r="P35">
+        <v>1352.450475948723</v>
+      </c>
+      <c r="Q35">
+        <v>0.586436963340958</v>
+      </c>
+      <c r="S35">
+        <v>2.106507142607232</v>
+      </c>
+      <c r="T35">
+        <v>0.2034227237052778</v>
+      </c>
+      <c r="U35">
+        <v>1.172873926681916</v>
+      </c>
+      <c r="V35" t="s">
+        <v>73</v>
+      </c>
+      <c r="W35">
+        <v>1266.358352471694</v>
+      </c>
+      <c r="X35">
+        <v>76.75589726916873</v>
+      </c>
+      <c r="Y35">
+        <v>0.6941470549936946</v>
+      </c>
+      <c r="Z35">
+        <v>1410.613724066265</v>
+      </c>
+      <c r="AA35">
+        <v>130.497972685586</v>
+      </c>
+      <c r="AB35">
+        <v>0.6042797213877116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31">
+      <c r="A36" s="1">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36">
+        <v>102.758897544719</v>
+      </c>
+      <c r="D36">
+        <v>1286.652539953465</v>
+      </c>
+      <c r="E36">
+        <v>516.7398857020447</v>
+      </c>
+      <c r="F36">
+        <v>1286.652589955965</v>
+      </c>
+      <c r="G36">
+        <v>708.9238504058497</v>
+      </c>
+      <c r="H36">
+        <v>0.6019901339660406</v>
+      </c>
+      <c r="I36">
+        <v>1.977679614020306</v>
+      </c>
+      <c r="J36">
+        <v>0.2043062100057697</v>
+      </c>
+      <c r="K36">
+        <v>1.203980267932081</v>
+      </c>
+      <c r="L36" t="s">
+        <v>73</v>
+      </c>
+      <c r="M36">
+        <v>1389.411537503184</v>
+      </c>
+      <c r="N36">
+        <v>791.7158397055947</v>
+      </c>
+      <c r="O36">
+        <v>1389.411487500684</v>
+      </c>
+      <c r="P36">
+        <v>1046.570016410767</v>
+      </c>
+      <c r="Q36">
+        <v>0.587550062841389</v>
+      </c>
+      <c r="S36">
+        <v>1.873244687270213</v>
+      </c>
+      <c r="T36">
+        <v>0.1667788947662797</v>
+      </c>
+      <c r="U36">
+        <v>1.175100125682778</v>
+      </c>
+      <c r="V36" t="s">
+        <v>73</v>
+      </c>
+      <c r="W36">
+        <v>1266.370895078406</v>
+      </c>
+      <c r="X36">
+        <v>59.80110225135093</v>
+      </c>
+      <c r="Y36">
+        <v>0.6480731510910379</v>
+      </c>
+      <c r="Z36">
+        <v>1410.642555440015</v>
+      </c>
+      <c r="AA36">
+        <v>95.84212254504136</v>
+      </c>
+      <c r="AB36">
+        <v>0.5882239754158175</v>
+      </c>
+      <c r="AC36">
+        <v>1371.209180767353</v>
+      </c>
+      <c r="AD36">
+        <v>17.69616686433925</v>
+      </c>
+      <c r="AE36">
+        <v>0.2934890726427765</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31">
+      <c r="A37" s="1">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37">
+        <v>102.7470021094227</v>
+      </c>
+      <c r="D37">
+        <v>1286.664023709264</v>
+      </c>
+      <c r="E37">
+        <v>369.8380629569173</v>
+      </c>
+      <c r="F37">
+        <v>1286.664023709264</v>
+      </c>
+      <c r="G37">
+        <v>491.8230261671195</v>
+      </c>
+      <c r="H37">
+        <v>0.6112809685653848</v>
+      </c>
+      <c r="I37">
+        <v>1.970989409887368</v>
+      </c>
+      <c r="J37">
+        <v>0.06638535155006831</v>
+      </c>
+      <c r="K37">
+        <v>1.22256193713077</v>
+      </c>
+      <c r="L37" t="s">
+        <v>73</v>
+      </c>
+      <c r="M37">
+        <v>1389.411075821187</v>
+      </c>
+      <c r="N37">
+        <v>579.3608148988537</v>
+      </c>
+      <c r="O37">
+        <v>1389.411025818687</v>
+      </c>
+      <c r="P37">
+        <v>763.9686354721808</v>
+      </c>
+      <c r="Q37">
+        <v>0.5816250205989264</v>
+      </c>
+      <c r="S37">
+        <v>1.925759599846889</v>
+      </c>
+      <c r="T37">
+        <v>0.1891939371367906</v>
+      </c>
+      <c r="U37">
+        <v>1.163250041197853</v>
+      </c>
+      <c r="V37" t="s">
+        <v>73</v>
+      </c>
+      <c r="W37">
+        <v>1266.349327991556</v>
+      </c>
+      <c r="X37">
+        <v>32.75052748262105</v>
+      </c>
+      <c r="Y37">
+        <v>0.5765000593824008</v>
+      </c>
+      <c r="Z37">
+        <v>1410.635182498057</v>
+      </c>
+      <c r="AA37">
+        <v>72.99060177586486</v>
+      </c>
+      <c r="AB37">
+        <v>0.5855542546116365</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31">
+      <c r="A38" s="1">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38">
+        <v>102.7260993368432</v>
+      </c>
+      <c r="D38">
+        <v>1286.691021976886</v>
+      </c>
+      <c r="E38">
+        <v>254.1827700593303</v>
+      </c>
+      <c r="F38">
+        <v>1286.691021976886</v>
+      </c>
+      <c r="G38">
+        <v>328.4633393189901</v>
+      </c>
+      <c r="H38">
+        <v>0.6068480416262925</v>
+      </c>
+      <c r="I38">
+        <v>1.962849028303957</v>
+      </c>
+      <c r="J38">
+        <v>0.000704490293250426</v>
+      </c>
+      <c r="K38">
+        <v>1.213696083252585</v>
+      </c>
+      <c r="L38" t="s">
+        <v>73</v>
+      </c>
+      <c r="M38">
+        <v>1389.41717131623</v>
+      </c>
+      <c r="N38">
+        <v>403.1331040072373</v>
+      </c>
+      <c r="O38">
+        <v>1389.417121313729</v>
+      </c>
+      <c r="P38">
+        <v>520.2692911297912</v>
+      </c>
+      <c r="Q38">
+        <v>0.5801466331330192</v>
+      </c>
+      <c r="S38">
+        <v>1.703450708405</v>
+      </c>
+      <c r="T38">
+        <v>0.1333485078806765</v>
+      </c>
+      <c r="U38">
+        <v>1.160293266266038</v>
+      </c>
+      <c r="V38" t="s">
+        <v>73</v>
+      </c>
+      <c r="W38">
+        <v>1266.36201929993</v>
+      </c>
+      <c r="X38">
+        <v>27.17553092235304</v>
+      </c>
+      <c r="Y38">
+        <v>0.64274010344903</v>
+      </c>
+      <c r="Z38">
+        <v>1410.681972010588</v>
+      </c>
+      <c r="AA38">
+        <v>48.5627408894663</v>
+      </c>
+      <c r="AB38">
+        <v>0.5945581659999187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31">
+      <c r="A39" s="1">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39">
+        <v>102.7402451923251</v>
+      </c>
+      <c r="D39">
+        <v>1286.697240683941</v>
+      </c>
+      <c r="E39">
+        <v>180.3320621001235</v>
+      </c>
+      <c r="F39">
+        <v>1286.697240683941</v>
+      </c>
+      <c r="G39">
+        <v>237.6938193560382</v>
+      </c>
+      <c r="H39">
+        <v>0.6156564190685897</v>
+      </c>
+      <c r="I39">
+        <v>2.542691889421866</v>
+      </c>
+      <c r="J39">
+        <v>0.01741161501309907</v>
+      </c>
+      <c r="K39">
+        <v>1.231312838137179</v>
+      </c>
+      <c r="L39" t="s">
+        <v>73</v>
+      </c>
+      <c r="M39">
+        <v>1389.437485876266</v>
+      </c>
+      <c r="N39">
+        <v>289.7880009581042</v>
+      </c>
+      <c r="O39">
+        <v>1389.437485876266</v>
+      </c>
+      <c r="P39">
+        <v>377.0007827554707</v>
+      </c>
+      <c r="Q39">
+        <v>0.582726049611217</v>
+      </c>
+      <c r="S39">
+        <v>2.364693939550456</v>
+      </c>
+      <c r="T39">
+        <v>0.1439576275270997</v>
+      </c>
+      <c r="U39">
+        <v>1.165452099222434</v>
+      </c>
+      <c r="V39" t="s">
+        <v>73</v>
+      </c>
+      <c r="W39">
+        <v>1266.356606469234</v>
+      </c>
+      <c r="X39">
+        <v>17.01643481827561</v>
+      </c>
+      <c r="Y39">
+        <v>0.5079452153840948</v>
+      </c>
+      <c r="Z39">
+        <v>1410.662305323734</v>
+      </c>
+      <c r="AA39">
+        <v>27.82347683178125</v>
+      </c>
+      <c r="AB39">
+        <v>0.5242435537051364</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31">
+      <c r="A40" s="1">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40">
+        <v>102.734128516593</v>
+      </c>
+      <c r="D40">
+        <v>1286.689608105534</v>
+      </c>
+      <c r="E40">
+        <v>244.9736880473542</v>
+      </c>
+      <c r="F40">
+        <v>1286.689608105534</v>
+      </c>
+      <c r="G40">
+        <v>309.7026757285485</v>
+      </c>
+      <c r="H40">
+        <v>0.5938193628948731</v>
+      </c>
+      <c r="I40">
+        <v>3.242024337086708</v>
+      </c>
+      <c r="J40">
+        <v>6.39637608791932E-05</v>
+      </c>
+      <c r="K40">
+        <v>1.187638725789746</v>
+      </c>
+      <c r="L40" t="s">
+        <v>73</v>
+      </c>
+      <c r="M40">
+        <v>1389.423786624628</v>
+      </c>
+      <c r="N40">
+        <v>387.276630841854</v>
+      </c>
+      <c r="O40">
+        <v>1389.423736622128</v>
+      </c>
+      <c r="P40">
+        <v>500.0061764243574</v>
+      </c>
+      <c r="Q40">
+        <v>0.5834588104829956</v>
+      </c>
+      <c r="S40">
+        <v>2.468755045442719</v>
+      </c>
+      <c r="T40">
+        <v>0.117590920776902</v>
+      </c>
+      <c r="U40">
+        <v>1.166917620965991</v>
+      </c>
+      <c r="V40" t="s">
+        <v>73</v>
+      </c>
+      <c r="W40">
+        <v>1266.095110302755</v>
+      </c>
+      <c r="X40">
+        <v>19.23975372240503</v>
+      </c>
+      <c r="Y40">
+        <v>0.6989055443704426</v>
+      </c>
+      <c r="Z40">
+        <v>1410.673321921606</v>
+      </c>
+      <c r="AA40">
+        <v>42.3187569527814</v>
+      </c>
+      <c r="AB40">
+        <v>0.5817867568000289</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31">
+      <c r="A41" s="1">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41">
+        <v>102.7610786908983</v>
+      </c>
+      <c r="D41">
+        <v>1286.675256972716</v>
+      </c>
+      <c r="E41">
+        <v>219.2687636623541</v>
+      </c>
+      <c r="F41">
+        <v>1286.675306975216</v>
+      </c>
+      <c r="G41">
+        <v>281.6102979574043</v>
+      </c>
+      <c r="H41">
+        <v>0.6029023052102631</v>
+      </c>
+      <c r="I41">
+        <v>5.73019064418228</v>
+      </c>
+      <c r="J41">
+        <v>0.001875364542617164</v>
+      </c>
+      <c r="K41">
+        <v>1.205804610420526</v>
+      </c>
+      <c r="L41" t="s">
+        <v>73</v>
+      </c>
+      <c r="M41">
+        <v>1389.436385666114</v>
+      </c>
+      <c r="N41">
+        <v>346.6613021637617</v>
+      </c>
+      <c r="O41">
+        <v>1389.436385666114</v>
+      </c>
+      <c r="P41">
+        <v>432.3159193333735</v>
+      </c>
+      <c r="Q41">
+        <v>0.5857737147394104</v>
+      </c>
+      <c r="S41">
+        <v>2.889239476325914</v>
+      </c>
+      <c r="T41">
+        <v>2.697441430399294E-05</v>
+      </c>
+      <c r="U41">
+        <v>1.171547429478821</v>
+      </c>
+      <c r="V41" t="s">
+        <v>73</v>
+      </c>
+      <c r="W41">
+        <v>1266.538485819774</v>
+      </c>
+      <c r="X41">
+        <v>16.75473498248556</v>
+      </c>
+      <c r="Y41">
+        <v>0.36194393083912</v>
+      </c>
+      <c r="Z41">
+        <v>1410.544648816307</v>
+      </c>
+      <c r="AA41">
+        <v>33.81123679889354</v>
+      </c>
+      <c r="AB41">
+        <v>0.481651204850689</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31">
+      <c r="A42" s="1">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42">
+        <v>102.7277060591155</v>
+      </c>
+      <c r="D42">
+        <v>1286.707689760344</v>
+      </c>
+      <c r="E42">
+        <v>155.7591743579446</v>
+      </c>
+      <c r="F42">
+        <v>1286.707689760344</v>
+      </c>
+      <c r="G42">
+        <v>208.1249559365736</v>
+      </c>
+      <c r="H42">
+        <v>0.6235608060643234</v>
+      </c>
+      <c r="I42">
+        <v>2.965047668134913</v>
+      </c>
+      <c r="J42">
+        <v>3.046736501977065E-08</v>
+      </c>
+      <c r="K42">
+        <v>1.247121612128647</v>
+      </c>
+      <c r="L42" t="s">
+        <v>73</v>
+      </c>
+      <c r="M42">
+        <v>1389.435395819459</v>
+      </c>
+      <c r="N42">
+        <v>264.1183842438014</v>
+      </c>
+      <c r="O42">
+        <v>1389.435395819459</v>
+      </c>
+      <c r="P42">
+        <v>321.3494653853786</v>
+      </c>
+      <c r="Q42">
+        <v>0.5715000684244254</v>
+      </c>
+      <c r="S42">
+        <v>2.650008792734035</v>
+      </c>
+      <c r="T42">
+        <v>3.250803074561492E-06</v>
+      </c>
+      <c r="U42">
+        <v>1.143000136848851</v>
+      </c>
+      <c r="V42" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z42">
+        <v>1410.700526720248</v>
+      </c>
+      <c r="AA42">
+        <v>22.42473067468594</v>
+      </c>
+      <c r="AB42">
+        <v>0.6065234816473117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31">
+      <c r="A43" s="1">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43">
+        <v>102.7305120710907</v>
+      </c>
+      <c r="D43">
+        <v>1286.713763863166</v>
+      </c>
+      <c r="E43">
+        <v>130.180532074986</v>
+      </c>
+      <c r="F43">
+        <v>1286.713813865666</v>
+      </c>
+      <c r="G43">
+        <v>168.1835479187667</v>
+      </c>
+      <c r="H43">
+        <v>0.6068412188464316</v>
+      </c>
+      <c r="I43">
+        <v>3.479940986776955</v>
+      </c>
+      <c r="J43">
+        <v>1.34224459419352E-06</v>
+      </c>
+      <c r="K43">
+        <v>1.213682437692863</v>
+      </c>
+      <c r="L43" t="s">
+        <v>73</v>
+      </c>
+      <c r="M43">
+        <v>1389.444375939257</v>
+      </c>
+      <c r="N43">
+        <v>233.3289597293797</v>
+      </c>
+      <c r="O43">
+        <v>1389.444325936757</v>
+      </c>
+      <c r="P43">
+        <v>284.1507128441351</v>
+      </c>
+      <c r="Q43">
+        <v>0.5200813470845763</v>
+      </c>
+      <c r="S43">
+        <v>2.806061129786361</v>
+      </c>
+      <c r="T43">
+        <v>0.2817300605742443</v>
+      </c>
+      <c r="U43">
+        <v>1.040162694169153</v>
+      </c>
+      <c r="V43" t="s">
+        <v>73</v>
+      </c>
+      <c r="W43">
+        <v>1266.472171567633</v>
+      </c>
+      <c r="X43">
+        <v>10.21902384745983</v>
+      </c>
+      <c r="Y43">
+        <v>0.3865478796841613</v>
+      </c>
+      <c r="Z43">
+        <v>1410.668572404536</v>
+      </c>
+      <c r="AA43">
+        <v>22.04781675749843</v>
+      </c>
+      <c r="AB43">
+        <v>0.525250754626383</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31">
+      <c r="A44" s="1">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44">
+        <v>102.7589230928222</v>
+      </c>
+      <c r="D44">
+        <v>1286.686840522868</v>
+      </c>
+      <c r="E44">
+        <v>125.4441478147111</v>
+      </c>
+      <c r="F44">
+        <v>1286.686840522868</v>
+      </c>
+      <c r="G44">
+        <v>154.1089831261463</v>
+      </c>
+      <c r="H44">
+        <v>0.5770525187632496</v>
+      </c>
+      <c r="I44">
+        <v>3.32524507613781</v>
+      </c>
+      <c r="J44">
+        <v>1.211610201057312E-09</v>
+      </c>
+      <c r="K44">
+        <v>1.154105037526499</v>
+      </c>
+      <c r="L44" t="s">
+        <v>73</v>
+      </c>
+      <c r="M44">
+        <v>1389.445813618191</v>
+      </c>
+      <c r="N44">
+        <v>191.3164696685896</v>
+      </c>
+      <c r="O44">
+        <v>1389.445763615691</v>
+      </c>
+      <c r="P44">
+        <v>485.4024173648132</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>6.172413044070529</v>
+      </c>
+      <c r="T44">
+        <v>0.5</v>
+      </c>
+      <c r="U44">
+        <v>2</v>
+      </c>
+      <c r="V44" t="s">
+        <v>73</v>
+      </c>
+      <c r="W44">
+        <v>1266.501341098302</v>
+      </c>
+      <c r="X44">
+        <v>7.755633165696673</v>
+      </c>
+      <c r="Y44">
+        <v>0.4654323476025005</v>
+      </c>
+      <c r="Z44">
+        <v>1409.300074</v>
+      </c>
+      <c r="AA44">
+        <v>267.0158974509757</v>
+      </c>
+      <c r="AB44">
+        <v>0.5662307984833664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>